<commit_message>
updated the indicators ID (added 'SIGI-')
</commit_message>
<xml_diff>
--- a/Simple_XLS_Importer/data/OECD-SIGI/OECD-SIGI-0.xlsx
+++ b/Simple_XLS_Importer/data/OECD-SIGI/OECD-SIGI-0.xlsx
@@ -1,17 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26819"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4507"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15540" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="11760" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
     <sheet name="metadata" sheetId="2" r:id="rId2"/>
     <sheet name="Statistical Metadata&amp;Notes" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="140000" concurrentCalc="0"/>
+  <calcPr calcId="125725" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="206">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="207">
   <si>
     <t>country</t>
   </si>
@@ -680,15 +680,18 @@
   <si>
     <t xml:space="preserve">  Zimbabwe</t>
   </si>
+  <si>
+    <t>SIGI-0</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="0.0000"/>
+    <numFmt numFmtId="164" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="4">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -756,10 +759,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1092,19 +1095,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C195"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D88" sqref="D88:D195"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.875" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="41.83203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.83203125" style="2"/>
+    <col min="1" max="1" width="41.875" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.875" style="2"/>
     <col min="3" max="3" width="35.5" style="7" bestFit="1" customWidth="1"/>
-    <col min="4" max="16384" width="10.83203125" style="2"/>
+    <col min="4" max="16384" width="10.875" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -3268,16 +3271,16 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="17.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -3301,8 +3304,8 @@
       <c r="A3" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="4">
-        <v>0</v>
+      <c r="B3" s="4" t="s">
+        <v>206</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -3324,14 +3327,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75"/>
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">

</xml_diff>

<commit_message>
Updated values for OECD-SIGI 2009 indicators
</commit_message>
<xml_diff>
--- a/Simple_XLS_Importer/data/OECD-SIGI/OECD-SIGI-0.xlsx
+++ b/Simple_XLS_Importer/data/OECD-SIGI/OECD-SIGI-0.xlsx
@@ -21,35 +21,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="207">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="309" uniqueCount="226">
   <si>
     <t>country</t>
   </si>
   <si>
     <t>year</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Note</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>: the 2009 version of SIGI is not retrievable anymore form the OECD site</t>
-    </r>
   </si>
   <si>
     <r>
@@ -681,6 +658,86 @@
     <t xml:space="preserve">  Zimbabwe</t>
   </si>
   <si>
+    <t xml:space="preserve">  Fiji</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Hong Kong, China</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Papua New Guinea</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Singapore</t>
+  </si>
+  <si>
+    <t>Chile</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Uruguay</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Croatia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Russia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Algeria</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Bahrain</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Iran</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Kuwait</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Libya</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  United Arab Emirates</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Botswana</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Côte d'Ivoire</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Equatorial Guinea</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Eritrea</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Mauritius</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Note</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>:Each wave of SIGI (2009, 2012, 2014) is different in terms of components and subcompontes of the SIGI index</t>
+    </r>
+  </si>
+  <si>
     <t>SIGI-0</t>
   </si>
 </sst>
@@ -691,7 +748,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="6">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -717,6 +774,22 @@
       <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -735,8 +808,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -766,7 +841,9 @@
       <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Hipervínculo" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1096,16 +1173,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C195"/>
+  <dimension ref="A1:C424"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D88" sqref="D88:D195"/>
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.875" defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="41.875" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.875" style="2"/>
+    <col min="2" max="2" width="22.375" style="2" customWidth="1"/>
     <col min="3" max="3" width="35.5" style="7" bestFit="1" customWidth="1"/>
     <col min="4" max="16384" width="10.875" style="2"/>
   </cols>
@@ -1118,2147 +1195,3647 @@
         <v>1</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="5" t="s">
-        <v>14</v>
+        <v>176</v>
       </c>
       <c r="B2" s="2">
-        <v>2012</v>
-      </c>
-      <c r="C2" s="8">
-        <v>6.8999999999999999E-3</v>
+        <v>2009</v>
+      </c>
+      <c r="C2" s="9">
+        <v>2.4832000000000001E-3</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="5" t="s">
-        <v>31</v>
+        <v>211</v>
       </c>
       <c r="B3" s="2">
-        <v>2012</v>
-      </c>
-      <c r="C3" s="8">
-        <v>2.1999999999999999E-2</v>
+        <v>2009</v>
+      </c>
+      <c r="C3" s="9">
+        <v>3.3300000000000001E-3</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="5" t="s">
-        <v>73</v>
+        <v>151</v>
       </c>
       <c r="B4" s="2">
-        <v>2012</v>
-      </c>
-      <c r="C4" s="8">
-        <v>6.4500000000000002E-2</v>
+        <v>2009</v>
+      </c>
+      <c r="C4" s="9">
+        <v>3.4778000000000001E-3</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="5" t="s">
-        <v>80</v>
+        <v>107</v>
       </c>
       <c r="B5" s="2">
-        <v>2012</v>
-      </c>
-      <c r="C5" s="8">
-        <v>0.10349999999999999</v>
+        <v>2009</v>
+      </c>
+      <c r="C5" s="9">
+        <v>3.7899000000000001E-3</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="5" t="s">
-        <v>39</v>
+        <v>128</v>
       </c>
       <c r="B6" s="2">
-        <v>2012</v>
-      </c>
-      <c r="C6" s="8">
-        <v>0.1047</v>
+        <v>2009</v>
+      </c>
+      <c r="C6" s="9">
+        <v>7.0933999999999997E-3</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" s="5" t="s">
-        <v>33</v>
+        <v>212</v>
       </c>
       <c r="B7" s="2">
-        <v>2012</v>
-      </c>
-      <c r="C7" s="8">
-        <v>0.1062</v>
+        <v>2009</v>
+      </c>
+      <c r="C7" s="9">
+        <v>7.2524E-3</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" s="5" t="s">
-        <v>89</v>
+        <v>178</v>
       </c>
       <c r="B8" s="2">
-        <v>2012</v>
-      </c>
-      <c r="C8" s="8">
-        <v>0.107</v>
+        <v>2009</v>
+      </c>
+      <c r="C8" s="9">
+        <v>7.8831000000000005E-3</v>
       </c>
     </row>
     <row r="9" spans="1:3">
       <c r="A9" s="5" t="s">
-        <v>22</v>
+        <v>134</v>
       </c>
       <c r="B9" s="2">
-        <v>2012</v>
-      </c>
-      <c r="C9" s="8">
-        <v>0.10920000000000001</v>
+        <v>2009</v>
+      </c>
+      <c r="C9" s="9">
+        <v>8.2581000000000009E-3</v>
       </c>
     </row>
     <row r="10" spans="1:3">
       <c r="A10" s="5" t="s">
-        <v>34</v>
+        <v>132</v>
       </c>
       <c r="B10" s="2">
-        <v>2012</v>
-      </c>
-      <c r="C10" s="8">
-        <v>0.11169999999999999</v>
+        <v>2009</v>
+      </c>
+      <c r="C10" s="9">
+        <v>9.1447000000000004E-3</v>
       </c>
     </row>
     <row r="11" spans="1:3">
       <c r="A11" s="5" t="s">
-        <v>37</v>
+        <v>198</v>
       </c>
       <c r="B11" s="2">
-        <v>2012</v>
-      </c>
-      <c r="C11" s="8">
-        <v>0.1158</v>
+        <v>2009</v>
+      </c>
+      <c r="C11" s="9">
+        <v>9.6900000000000007E-3</v>
       </c>
     </row>
     <row r="12" spans="1:3">
       <c r="A12" s="5" t="s">
-        <v>77</v>
+        <v>223</v>
       </c>
       <c r="B12" s="2">
-        <v>2012</v>
-      </c>
-      <c r="C12" s="8">
-        <v>0.11799999999999999</v>
+        <v>2009</v>
+      </c>
+      <c r="C12" s="9">
+        <v>9.7590000000000003E-3</v>
       </c>
     </row>
     <row r="13" spans="1:3">
       <c r="A13" s="5" t="s">
-        <v>74</v>
+        <v>164</v>
       </c>
       <c r="B13" s="2">
-        <v>2012</v>
-      </c>
-      <c r="C13" s="8">
-        <v>0.12</v>
+        <v>2009</v>
+      </c>
+      <c r="C13" s="9">
+        <v>9.8034999999999997E-3</v>
       </c>
     </row>
     <row r="14" spans="1:3">
       <c r="A14" s="5" t="s">
-        <v>25</v>
+        <v>114</v>
       </c>
       <c r="B14" s="2">
-        <v>2012</v>
-      </c>
-      <c r="C14" s="8">
-        <v>0.12130000000000001</v>
+        <v>2009</v>
+      </c>
+      <c r="C14" s="9">
+        <v>9.8346000000000006E-3</v>
       </c>
     </row>
     <row r="15" spans="1:3">
       <c r="A15" s="5" t="s">
-        <v>53</v>
+        <v>210</v>
       </c>
       <c r="B15" s="2">
-        <v>2012</v>
-      </c>
-      <c r="C15" s="8">
-        <v>0.122</v>
+        <v>2009</v>
+      </c>
+      <c r="C15" s="9">
+        <v>9.9167000000000005E-3</v>
       </c>
     </row>
     <row r="16" spans="1:3">
       <c r="A16" s="5" t="s">
-        <v>18</v>
+        <v>200</v>
       </c>
       <c r="B16" s="2">
-        <v>2012</v>
-      </c>
-      <c r="C16" s="8">
-        <v>0.12570000000000001</v>
+        <v>2009</v>
+      </c>
+      <c r="C16" s="9">
+        <v>1.04259E-2</v>
       </c>
     </row>
     <row r="17" spans="1:3">
       <c r="A17" s="5" t="s">
-        <v>94</v>
+        <v>192</v>
       </c>
       <c r="B17" s="2">
-        <v>2012</v>
-      </c>
-      <c r="C17" s="8">
-        <v>0.1258</v>
+        <v>2009</v>
+      </c>
+      <c r="C17" s="9">
+        <v>1.0677000000000001E-2</v>
       </c>
     </row>
     <row r="18" spans="1:3">
       <c r="A18" s="5" t="s">
-        <v>64</v>
+        <v>177</v>
       </c>
       <c r="B18" s="2">
-        <v>2012</v>
-      </c>
-      <c r="C18" s="8">
-        <v>0.12670000000000001</v>
+        <v>2009</v>
+      </c>
+      <c r="C18" s="9">
+        <v>1.21323E-2</v>
       </c>
     </row>
     <row r="19" spans="1:3">
       <c r="A19" s="5" t="s">
-        <v>48</v>
+        <v>125</v>
       </c>
       <c r="B19" s="2">
-        <v>2012</v>
-      </c>
-      <c r="C19" s="8">
-        <v>0.13109999999999999</v>
+        <v>2009</v>
+      </c>
+      <c r="C19" s="9">
+        <v>1.2727E-2</v>
       </c>
     </row>
     <row r="20" spans="1:3">
       <c r="A20" s="5" t="s">
-        <v>35</v>
+        <v>111</v>
       </c>
       <c r="B20" s="2">
-        <v>2012</v>
-      </c>
-      <c r="C20" s="8">
-        <v>0.13139999999999999</v>
+        <v>2009</v>
+      </c>
+      <c r="C20" s="9">
+        <v>1.3385599999999999E-2</v>
       </c>
     </row>
     <row r="21" spans="1:3">
       <c r="A21" s="5" t="s">
-        <v>20</v>
+        <v>206</v>
       </c>
       <c r="B21" s="2">
-        <v>2012</v>
-      </c>
-      <c r="C21" s="8">
-        <v>0.1336</v>
+        <v>2009</v>
+      </c>
+      <c r="C21" s="9">
+        <v>1.46549E-2</v>
       </c>
     </row>
     <row r="22" spans="1:3">
       <c r="A22" s="5" t="s">
-        <v>67</v>
+        <v>208</v>
       </c>
       <c r="B22" s="2">
-        <v>2012</v>
-      </c>
-      <c r="C22" s="8">
-        <v>0.1358</v>
+        <v>2009</v>
+      </c>
+      <c r="C22" s="9">
+        <v>1.52573E-2</v>
       </c>
     </row>
     <row r="23" spans="1:3">
       <c r="A23" s="5" t="s">
-        <v>90</v>
+        <v>130</v>
       </c>
       <c r="B23" s="2">
-        <v>2012</v>
-      </c>
-      <c r="C23" s="8">
-        <v>0.13589999999999999</v>
+        <v>2009</v>
+      </c>
+      <c r="C23" s="9">
+        <v>1.60304E-2</v>
       </c>
     </row>
     <row r="24" spans="1:3">
       <c r="A24" s="5" t="s">
-        <v>63</v>
+        <v>136</v>
       </c>
       <c r="B24" s="2">
-        <v>2012</v>
-      </c>
-      <c r="C24" s="8">
-        <v>0.14299999999999999</v>
+        <v>2009</v>
+      </c>
+      <c r="C24" s="9">
+        <v>1.7869599999999999E-2</v>
       </c>
     </row>
     <row r="25" spans="1:3">
       <c r="A25" s="5" t="s">
-        <v>21</v>
+        <v>116</v>
       </c>
       <c r="B25" s="2">
-        <v>2012</v>
-      </c>
-      <c r="C25" s="8">
-        <v>0.14330000000000001</v>
+        <v>2009</v>
+      </c>
+      <c r="C25" s="9">
+        <v>1.8802099999999999E-2</v>
       </c>
     </row>
     <row r="26" spans="1:3">
       <c r="A26" s="5" t="s">
-        <v>87</v>
+        <v>196</v>
       </c>
       <c r="B26" s="2">
-        <v>2012</v>
-      </c>
-      <c r="C26" s="8">
-        <v>0.14749999999999999</v>
+        <v>2009</v>
+      </c>
+      <c r="C26" s="9">
+        <v>1.90618E-2</v>
       </c>
     </row>
     <row r="27" spans="1:3">
       <c r="A27" s="5" t="s">
-        <v>29</v>
+        <v>209</v>
       </c>
       <c r="B27" s="2">
-        <v>2012</v>
-      </c>
-      <c r="C27" s="8">
-        <v>0.1477</v>
+        <v>2009</v>
+      </c>
+      <c r="C27" s="9">
+        <v>1.95128E-2</v>
       </c>
     </row>
     <row r="28" spans="1:3">
       <c r="A28" s="5" t="s">
-        <v>92</v>
+        <v>120</v>
       </c>
       <c r="B28" s="2">
-        <v>2012</v>
-      </c>
-      <c r="C28" s="8">
-        <v>0.1522</v>
+        <v>2009</v>
+      </c>
+      <c r="C28" s="9">
+        <v>2.2018800000000002E-2</v>
       </c>
     </row>
     <row r="29" spans="1:3">
       <c r="A29" s="5" t="s">
-        <v>75</v>
+        <v>171</v>
       </c>
       <c r="B29" s="2">
-        <v>2012</v>
-      </c>
-      <c r="C29" s="8">
-        <v>0.15429999999999999</v>
+        <v>2009</v>
+      </c>
+      <c r="C29" s="9">
+        <v>2.2514900000000001E-2</v>
       </c>
     </row>
     <row r="30" spans="1:3">
       <c r="A30" s="5" t="s">
-        <v>62</v>
+        <v>195</v>
       </c>
       <c r="B30" s="2">
-        <v>2012</v>
-      </c>
-      <c r="C30" s="8">
-        <v>0.16020000000000001</v>
+        <v>2009</v>
+      </c>
+      <c r="C30" s="9">
+        <v>2.2881499999999999E-2</v>
       </c>
     </row>
     <row r="31" spans="1:3">
       <c r="A31" s="5" t="s">
-        <v>58</v>
+        <v>153</v>
       </c>
       <c r="B31" s="2">
-        <v>2012</v>
-      </c>
-      <c r="C31" s="8">
-        <v>0.16789999999999999</v>
+        <v>2009</v>
+      </c>
+      <c r="C31" s="9">
+        <v>2.9241900000000001E-2</v>
       </c>
     </row>
     <row r="32" spans="1:3">
       <c r="A32" s="5" t="s">
-        <v>47</v>
+        <v>201</v>
       </c>
       <c r="B32" s="2">
-        <v>2012</v>
-      </c>
-      <c r="C32" s="8">
-        <v>0.16980000000000001</v>
+        <v>2009</v>
+      </c>
+      <c r="C32" s="9">
+        <v>3.0061899999999999E-2</v>
       </c>
     </row>
     <row r="33" spans="1:3">
       <c r="A33" s="5" t="s">
-        <v>50</v>
+        <v>108</v>
       </c>
       <c r="B33" s="2">
-        <v>2012</v>
-      </c>
-      <c r="C33" s="8">
-        <v>0.17430000000000001</v>
+        <v>2009</v>
+      </c>
+      <c r="C33" s="9">
+        <v>3.0117700000000001E-2</v>
       </c>
     </row>
     <row r="34" spans="1:3">
       <c r="A34" s="5" t="s">
-        <v>55</v>
+        <v>139</v>
       </c>
       <c r="B34" s="2">
-        <v>2012</v>
-      </c>
-      <c r="C34" s="8">
-        <v>0.17610000000000001</v>
+        <v>2009</v>
+      </c>
+      <c r="C34" s="9">
+        <v>3.06926E-2</v>
       </c>
     </row>
     <row r="35" spans="1:3">
       <c r="A35" s="5" t="s">
-        <v>52</v>
+        <v>141</v>
       </c>
       <c r="B35" s="2">
-        <v>2012</v>
-      </c>
-      <c r="C35" s="8">
-        <v>0.2077</v>
+        <v>2009</v>
+      </c>
+      <c r="C35" s="9">
+        <v>3.19271E-2</v>
       </c>
     </row>
     <row r="36" spans="1:3">
       <c r="A36" s="5" t="s">
-        <v>44</v>
+        <v>190</v>
       </c>
       <c r="B36" s="2">
-        <v>2012</v>
-      </c>
-      <c r="C36" s="8">
-        <v>0.21279999999999999</v>
+        <v>2009</v>
+      </c>
+      <c r="C36" s="9">
+        <v>3.2623699999999999E-2</v>
       </c>
     </row>
     <row r="37" spans="1:3">
       <c r="A37" s="5" t="s">
-        <v>68</v>
+        <v>145</v>
       </c>
       <c r="B37" s="2">
-        <v>2012</v>
-      </c>
-      <c r="C37" s="8">
-        <v>0.21540000000000001</v>
+        <v>2009</v>
+      </c>
+      <c r="C37" s="9">
+        <v>3.3162499999999998E-2</v>
       </c>
     </row>
     <row r="38" spans="1:3">
       <c r="A38" s="5" t="s">
-        <v>69</v>
+        <v>109</v>
       </c>
       <c r="B38" s="2">
-        <v>2012</v>
-      </c>
-      <c r="C38" s="8">
-        <v>0.2167</v>
+        <v>2009</v>
+      </c>
+      <c r="C38" s="9">
+        <v>3.3949600000000003E-2</v>
       </c>
     </row>
     <row r="39" spans="1:3">
       <c r="A39" s="5" t="s">
-        <v>59</v>
+        <v>154</v>
       </c>
       <c r="B39" s="2">
-        <v>2012</v>
-      </c>
-      <c r="C39" s="8">
-        <v>0.21779999999999999</v>
+        <v>2009</v>
+      </c>
+      <c r="C39" s="9">
+        <v>3.57687E-2</v>
       </c>
     </row>
     <row r="40" spans="1:3">
       <c r="A40" s="5" t="s">
-        <v>65</v>
+        <v>165</v>
       </c>
       <c r="B40" s="2">
-        <v>2012</v>
-      </c>
-      <c r="C40" s="8">
-        <v>0.22</v>
+        <v>2009</v>
+      </c>
+      <c r="C40" s="9">
+        <v>3.9116499999999998E-2</v>
       </c>
     </row>
     <row r="41" spans="1:3">
       <c r="A41" s="5" t="s">
-        <v>85</v>
+        <v>131</v>
       </c>
       <c r="B41" s="2">
-        <v>2012</v>
-      </c>
-      <c r="C41" s="8">
-        <v>0.22459999999999999</v>
+        <v>2009</v>
+      </c>
+      <c r="C41" s="9">
+        <v>3.9837900000000002E-2</v>
       </c>
     </row>
     <row r="42" spans="1:3">
       <c r="A42" s="5" t="s">
-        <v>76</v>
+        <v>168</v>
       </c>
       <c r="B42" s="2">
-        <v>2012</v>
-      </c>
-      <c r="C42" s="8">
-        <v>0.23039999999999999</v>
+        <v>2009</v>
+      </c>
+      <c r="C42" s="9">
+        <v>4.6287099999999998E-2</v>
       </c>
     </row>
     <row r="43" spans="1:3">
       <c r="A43" s="5" t="s">
-        <v>28</v>
+        <v>149</v>
       </c>
       <c r="B43" s="2">
-        <v>2012</v>
-      </c>
-      <c r="C43" s="8">
-        <v>0.23880000000000001</v>
+        <v>2009</v>
+      </c>
+      <c r="C43" s="9">
+        <v>4.8429300000000002E-2</v>
       </c>
     </row>
     <row r="44" spans="1:3">
       <c r="A44" s="5" t="s">
-        <v>95</v>
+        <v>166</v>
       </c>
       <c r="B44" s="2">
-        <v>2012</v>
-      </c>
-      <c r="C44" s="8">
-        <v>0.23930000000000001</v>
+        <v>2009</v>
+      </c>
+      <c r="C44" s="9">
+        <v>5.34361E-2</v>
       </c>
     </row>
     <row r="45" spans="1:3">
       <c r="A45" s="5" t="s">
-        <v>66</v>
+        <v>205</v>
       </c>
       <c r="B45" s="2">
-        <v>2012</v>
-      </c>
-      <c r="C45" s="8">
-        <v>0.24049999999999999</v>
+        <v>2009</v>
+      </c>
+      <c r="C45" s="9">
+        <v>5.4504400000000001E-2</v>
       </c>
     </row>
     <row r="46" spans="1:3">
       <c r="A46" s="5" t="s">
-        <v>46</v>
+        <v>186</v>
       </c>
       <c r="B46" s="2">
-        <v>2012</v>
-      </c>
-      <c r="C46" s="8">
-        <v>0.24429999999999999</v>
+        <v>2009</v>
+      </c>
+      <c r="C46" s="9">
+        <v>5.9140999999999999E-2</v>
       </c>
     </row>
     <row r="47" spans="1:3">
       <c r="A47" s="5" t="s">
-        <v>54</v>
+        <v>160</v>
       </c>
       <c r="B47" s="2">
-        <v>2012</v>
-      </c>
-      <c r="C47" s="8">
-        <v>0.2487</v>
+        <v>2009</v>
+      </c>
+      <c r="C47" s="9">
+        <v>6.9581500000000004E-2</v>
       </c>
     </row>
     <row r="48" spans="1:3">
       <c r="A48" s="5" t="s">
-        <v>86</v>
+        <v>169</v>
       </c>
       <c r="B48" s="2">
-        <v>2012</v>
-      </c>
-      <c r="C48" s="8">
-        <v>0.25209999999999999</v>
+        <v>2009</v>
+      </c>
+      <c r="C48" s="9">
+        <v>7.5023699999999999E-2</v>
       </c>
     </row>
     <row r="49" spans="1:3">
       <c r="A49" s="5" t="s">
-        <v>61</v>
+        <v>219</v>
       </c>
       <c r="B49" s="2">
-        <v>2012</v>
-      </c>
-      <c r="C49" s="8">
-        <v>0.2545</v>
+        <v>2009</v>
+      </c>
+      <c r="C49" s="9">
+        <v>8.1017199999999998E-2</v>
       </c>
     </row>
     <row r="50" spans="1:3">
       <c r="A50" s="5" t="s">
-        <v>56</v>
+        <v>185</v>
       </c>
       <c r="B50" s="2">
-        <v>2012</v>
-      </c>
-      <c r="C50" s="8">
-        <v>0.25990000000000002</v>
+        <v>2009</v>
+      </c>
+      <c r="C50" s="9">
+        <v>8.6768899999999996E-2</v>
       </c>
     </row>
     <row r="51" spans="1:3">
       <c r="A51" s="5" t="s">
-        <v>43</v>
+        <v>119</v>
       </c>
       <c r="B51" s="2">
-        <v>2012</v>
-      </c>
-      <c r="C51" s="8">
-        <v>0.26219999999999999</v>
+        <v>2009</v>
+      </c>
+      <c r="C51" s="9">
+        <v>0.1069056</v>
       </c>
     </row>
     <row r="52" spans="1:3">
       <c r="A52" s="5" t="s">
-        <v>24</v>
+        <v>105</v>
       </c>
       <c r="B52" s="2">
-        <v>2012</v>
-      </c>
-      <c r="C52" s="8">
-        <v>0.27550000000000002</v>
+        <v>2009</v>
+      </c>
+      <c r="C52" s="9">
+        <v>0.1071956</v>
       </c>
     </row>
     <row r="53" spans="1:3">
       <c r="A53" s="5" t="s">
-        <v>13</v>
+        <v>181</v>
       </c>
       <c r="B53" s="2">
-        <v>2012</v>
-      </c>
-      <c r="C53" s="8">
-        <v>0.27929999999999999</v>
+        <v>2009</v>
+      </c>
+      <c r="C53" s="9">
+        <v>0.11040560000000001</v>
       </c>
     </row>
     <row r="54" spans="1:3">
       <c r="A54" s="5" t="s">
-        <v>81</v>
+        <v>191</v>
       </c>
       <c r="B54" s="2">
-        <v>2012</v>
-      </c>
-      <c r="C54" s="8">
-        <v>0.27979999999999999</v>
+        <v>2009</v>
+      </c>
+      <c r="C54" s="9">
+        <v>0.1124419</v>
       </c>
     </row>
     <row r="55" spans="1:3">
       <c r="A55" s="5" t="s">
-        <v>15</v>
+        <v>140</v>
       </c>
       <c r="B55" s="2">
-        <v>2012</v>
-      </c>
-      <c r="C55" s="8">
-        <v>0.28539999999999999</v>
+        <v>2009</v>
+      </c>
+      <c r="C55" s="9">
+        <v>0.112694</v>
       </c>
     </row>
     <row r="56" spans="1:3">
       <c r="A56" s="5" t="s">
-        <v>72</v>
+        <v>147</v>
       </c>
       <c r="B56" s="2">
-        <v>2012</v>
-      </c>
-      <c r="C56" s="8">
-        <v>0.29339999999999999</v>
+        <v>2009</v>
+      </c>
+      <c r="C56" s="9">
+        <v>0.12776090000000001</v>
       </c>
     </row>
     <row r="57" spans="1:3">
       <c r="A57" s="5" t="s">
-        <v>49</v>
+        <v>222</v>
       </c>
       <c r="B57" s="2">
-        <v>2012</v>
-      </c>
-      <c r="C57" s="8">
-        <v>0.30470000000000003</v>
+        <v>2009</v>
+      </c>
+      <c r="C57" s="9">
+        <v>0.13644690000000001</v>
       </c>
     </row>
     <row r="58" spans="1:3">
       <c r="A58" s="5" t="s">
-        <v>93</v>
+        <v>152</v>
       </c>
       <c r="B58" s="2">
-        <v>2012</v>
-      </c>
-      <c r="C58" s="8">
-        <v>0.30470000000000003</v>
+        <v>2009</v>
+      </c>
+      <c r="C58" s="9">
+        <v>0.13704160000000001</v>
       </c>
     </row>
     <row r="59" spans="1:3">
       <c r="A59" s="5" t="s">
-        <v>97</v>
+        <v>220</v>
       </c>
       <c r="B59" s="2">
-        <v>2012</v>
-      </c>
-      <c r="C59" s="8">
-        <v>0.30499999999999999</v>
+        <v>2009</v>
+      </c>
+      <c r="C59" s="9">
+        <v>0.13711809999999999</v>
       </c>
     </row>
     <row r="60" spans="1:3">
       <c r="A60" s="5" t="s">
-        <v>51</v>
+        <v>189</v>
       </c>
       <c r="B60" s="2">
-        <v>2012</v>
-      </c>
-      <c r="C60" s="8">
-        <v>0.3175</v>
+        <v>2009</v>
+      </c>
+      <c r="C60" s="9">
+        <v>0.1381059</v>
       </c>
     </row>
     <row r="61" spans="1:3">
       <c r="A61" s="5" t="s">
-        <v>42</v>
+        <v>161</v>
       </c>
       <c r="B61" s="2">
-        <v>2012</v>
-      </c>
-      <c r="C61" s="8">
-        <v>0.3382</v>
+        <v>2009</v>
+      </c>
+      <c r="C61" s="9">
+        <v>0.1432271</v>
       </c>
     </row>
     <row r="62" spans="1:3">
       <c r="A62" s="5" t="s">
-        <v>32</v>
+        <v>163</v>
       </c>
       <c r="B62" s="2">
-        <v>2012</v>
-      </c>
-      <c r="C62" s="8">
-        <v>0.3402</v>
+        <v>2009</v>
+      </c>
+      <c r="C62" s="9">
+        <v>0.14970320000000001</v>
       </c>
     </row>
     <row r="63" spans="1:3">
       <c r="A63" s="5" t="s">
-        <v>57</v>
+        <v>188</v>
       </c>
       <c r="B63" s="2">
-        <v>2012</v>
-      </c>
-      <c r="C63" s="8">
-        <v>0.34420000000000001</v>
+        <v>2009</v>
+      </c>
+      <c r="C63" s="9">
+        <v>0.15654989999999999</v>
       </c>
     </row>
     <row r="64" spans="1:3">
       <c r="A64" s="5" t="s">
-        <v>17</v>
+        <v>118</v>
       </c>
       <c r="B64" s="2">
-        <v>2012</v>
-      </c>
-      <c r="C64" s="8">
-        <v>0.35239999999999999</v>
+        <v>2009</v>
+      </c>
+      <c r="C64" s="9">
+        <v>0.1616069</v>
       </c>
     </row>
     <row r="65" spans="1:3">
       <c r="A65" s="5" t="s">
-        <v>38</v>
+        <v>113</v>
       </c>
       <c r="B65" s="2">
-        <v>2012</v>
-      </c>
-      <c r="C65" s="8">
-        <v>0.35360000000000003</v>
+        <v>2009</v>
+      </c>
+      <c r="C65" s="9">
+        <v>0.16250800000000001</v>
       </c>
     </row>
     <row r="66" spans="1:3">
       <c r="A66" s="5" t="s">
-        <v>36</v>
+        <v>170</v>
       </c>
       <c r="B66" s="2">
-        <v>2012</v>
-      </c>
-      <c r="C66" s="8">
-        <v>0.35780000000000001</v>
+        <v>2009</v>
+      </c>
+      <c r="C66" s="9">
+        <v>0.16722519999999999</v>
       </c>
     </row>
     <row r="67" spans="1:3">
       <c r="A67" s="5" t="s">
-        <v>78</v>
+        <v>180</v>
       </c>
       <c r="B67" s="2">
-        <v>2012</v>
-      </c>
-      <c r="C67" s="8">
-        <v>0.36099999999999999</v>
+        <v>2009</v>
+      </c>
+      <c r="C67" s="9">
+        <v>0.16858590000000001</v>
       </c>
     </row>
     <row r="68" spans="1:3">
       <c r="A68" s="5" t="s">
-        <v>88</v>
+        <v>172</v>
       </c>
       <c r="B68" s="2">
-        <v>2012</v>
-      </c>
-      <c r="C68" s="8">
-        <v>0.36120000000000002</v>
+        <v>2009</v>
+      </c>
+      <c r="C68" s="9">
+        <v>0.1755873</v>
       </c>
     </row>
     <row r="69" spans="1:3">
       <c r="A69" s="5" t="s">
-        <v>16</v>
+        <v>221</v>
       </c>
       <c r="B69" s="2">
-        <v>2012</v>
-      </c>
-      <c r="C69" s="8">
-        <v>0.36249999999999999</v>
+        <v>2009</v>
+      </c>
+      <c r="C69" s="9">
+        <v>0.17597189999999999</v>
       </c>
     </row>
     <row r="70" spans="1:3">
       <c r="A70" s="5" t="s">
-        <v>12</v>
+        <v>138</v>
       </c>
       <c r="B70" s="2">
-        <v>2012</v>
-      </c>
-      <c r="C70" s="8">
-        <v>0.36309999999999998</v>
+        <v>2009</v>
+      </c>
+      <c r="C70" s="9">
+        <v>0.17829780000000001</v>
       </c>
     </row>
     <row r="71" spans="1:3">
       <c r="A71" s="5" t="s">
-        <v>23</v>
+        <v>122</v>
       </c>
       <c r="B71" s="2">
-        <v>2012</v>
-      </c>
-      <c r="C71" s="8">
-        <v>0.36919999999999997</v>
+        <v>2009</v>
+      </c>
+      <c r="C71" s="9">
+        <v>0.18439729999999999</v>
       </c>
     </row>
     <row r="72" spans="1:3">
       <c r="A72" s="5" t="s">
-        <v>26</v>
+        <v>216</v>
       </c>
       <c r="B72" s="2">
-        <v>2012</v>
-      </c>
-      <c r="C72" s="8">
-        <v>0.37059999999999998</v>
+        <v>2009</v>
+      </c>
+      <c r="C72" s="9">
+        <v>0.1860213</v>
       </c>
     </row>
     <row r="73" spans="1:3">
       <c r="A73" s="5" t="s">
-        <v>70</v>
+        <v>204</v>
       </c>
       <c r="B73" s="2">
-        <v>2012</v>
-      </c>
-      <c r="C73" s="8">
-        <v>0.37219999999999998</v>
+        <v>2009</v>
+      </c>
+      <c r="C73" s="9">
+        <v>0.18699579999999999</v>
       </c>
     </row>
     <row r="74" spans="1:3">
       <c r="A74" s="5" t="s">
-        <v>91</v>
+        <v>197</v>
       </c>
       <c r="B74" s="2">
-        <v>2012</v>
-      </c>
-      <c r="C74" s="8">
-        <v>0.3836</v>
+        <v>2009</v>
+      </c>
+      <c r="C74" s="9">
+        <v>0.1871794</v>
       </c>
     </row>
     <row r="75" spans="1:3">
       <c r="A75" s="5" t="s">
-        <v>83</v>
+        <v>112</v>
       </c>
       <c r="B75" s="2">
-        <v>2012</v>
-      </c>
-      <c r="C75" s="8">
-        <v>0.39150000000000001</v>
+        <v>2009</v>
+      </c>
+      <c r="C75" s="9">
+        <v>0.18899450000000001</v>
       </c>
     </row>
     <row r="76" spans="1:3">
       <c r="A76" s="5" t="s">
-        <v>84</v>
+        <v>213</v>
       </c>
       <c r="B76" s="2">
-        <v>2012</v>
-      </c>
-      <c r="C76" s="8">
-        <v>0.39279999999999998</v>
+        <v>2009</v>
+      </c>
+      <c r="C76" s="9">
+        <v>0.190244</v>
       </c>
     </row>
     <row r="77" spans="1:3">
       <c r="A77" s="5" t="s">
-        <v>41</v>
+        <v>214</v>
       </c>
       <c r="B77" s="2">
-        <v>2012</v>
-      </c>
-      <c r="C77" s="8">
-        <v>0.3947</v>
+        <v>2009</v>
+      </c>
+      <c r="C77" s="9">
+        <v>0.19654759999999999</v>
       </c>
     </row>
     <row r="78" spans="1:3">
       <c r="A78" s="5" t="s">
-        <v>40</v>
+        <v>167</v>
       </c>
       <c r="B78" s="2">
-        <v>2012</v>
-      </c>
-      <c r="C78" s="8">
-        <v>0.4289</v>
+        <v>2009</v>
+      </c>
+      <c r="C78" s="9">
+        <v>0.1995442</v>
       </c>
     </row>
     <row r="79" spans="1:3">
       <c r="A79" s="5" t="s">
-        <v>45</v>
+        <v>194</v>
       </c>
       <c r="B79" s="2">
-        <v>2012</v>
-      </c>
-      <c r="C79" s="8">
-        <v>0.44009999999999999</v>
+        <v>2009</v>
+      </c>
+      <c r="C79" s="9">
+        <v>0.202518</v>
       </c>
     </row>
     <row r="80" spans="1:3">
       <c r="A80" s="5" t="s">
-        <v>71</v>
+        <v>127</v>
       </c>
       <c r="B80" s="2">
-        <v>2012</v>
-      </c>
-      <c r="C80" s="8">
-        <v>0.44219999999999998</v>
+        <v>2009</v>
+      </c>
+      <c r="C80" s="9">
+        <v>0.20448169999999999</v>
       </c>
     </row>
     <row r="81" spans="1:3">
       <c r="A81" s="5" t="s">
-        <v>27</v>
+        <v>207</v>
       </c>
       <c r="B81" s="2">
-        <v>2012</v>
-      </c>
-      <c r="C81" s="8">
-        <v>0.45300000000000001</v>
+        <v>2009</v>
+      </c>
+      <c r="C81" s="9">
+        <v>0.20935790000000001</v>
       </c>
     </row>
     <row r="82" spans="1:3">
       <c r="A82" s="5" t="s">
-        <v>19</v>
+        <v>121</v>
       </c>
       <c r="B82" s="2">
-        <v>2012</v>
-      </c>
-      <c r="C82" s="8">
-        <v>0.45669999999999999</v>
+        <v>2009</v>
+      </c>
+      <c r="C82" s="9">
+        <v>0.21651210000000001</v>
       </c>
     </row>
     <row r="83" spans="1:3">
       <c r="A83" s="5" t="s">
-        <v>79</v>
+        <v>133</v>
       </c>
       <c r="B83" s="2">
-        <v>2012</v>
-      </c>
-      <c r="C83" s="8">
-        <v>0.49919999999999998</v>
+        <v>2009</v>
+      </c>
+      <c r="C83" s="9">
+        <v>0.21766079999999999</v>
       </c>
     </row>
     <row r="84" spans="1:3">
       <c r="A84" s="5" t="s">
-        <v>96</v>
+        <v>124</v>
       </c>
       <c r="B84" s="2">
-        <v>2012</v>
-      </c>
-      <c r="C84" s="8">
-        <v>0.50619999999999998</v>
+        <v>2009</v>
+      </c>
+      <c r="C84" s="9">
+        <v>0.21785589999999999</v>
       </c>
     </row>
     <row r="85" spans="1:3">
       <c r="A85" s="5" t="s">
-        <v>30</v>
+        <v>137</v>
       </c>
       <c r="B85" s="2">
-        <v>2012</v>
-      </c>
-      <c r="C85" s="8">
-        <v>0.51339999999999997</v>
+        <v>2009</v>
+      </c>
+      <c r="C85" s="9">
+        <v>0.21892239999999999</v>
       </c>
     </row>
     <row r="86" spans="1:3">
       <c r="A86" s="5" t="s">
-        <v>82</v>
+        <v>203</v>
       </c>
       <c r="B86" s="2">
-        <v>2012</v>
-      </c>
-      <c r="C86" s="8">
-        <v>0.52459999999999996</v>
+        <v>2009</v>
+      </c>
+      <c r="C86" s="9">
+        <v>0.21938759999999999</v>
       </c>
     </row>
     <row r="87" spans="1:3">
       <c r="A87" s="5" t="s">
-        <v>60</v>
+        <v>173</v>
       </c>
       <c r="B87" s="2">
-        <v>2012</v>
-      </c>
-      <c r="C87" s="8">
-        <v>0.60109999999999997</v>
+        <v>2009</v>
+      </c>
+      <c r="C87" s="9">
+        <v>0.2199123</v>
       </c>
     </row>
     <row r="88" spans="1:3">
       <c r="A88" s="5" t="s">
-        <v>98</v>
+        <v>158</v>
       </c>
       <c r="B88" s="2">
-        <v>2014</v>
+        <v>2009</v>
       </c>
       <c r="C88" s="9">
-        <v>1.6000000000000001E-3</v>
+        <v>0.2265095</v>
       </c>
     </row>
     <row r="89" spans="1:3">
       <c r="A89" s="5" t="s">
-        <v>100</v>
+        <v>142</v>
       </c>
       <c r="B89" s="2">
-        <v>2014</v>
+        <v>2009</v>
       </c>
       <c r="C89" s="9">
-        <v>3.3999999999999998E-3</v>
+        <v>0.22802929999999999</v>
       </c>
     </row>
     <row r="90" spans="1:3">
       <c r="A90" s="5" t="s">
-        <v>102</v>
+        <v>135</v>
       </c>
       <c r="B90" s="2">
-        <v>2014</v>
+        <v>2009</v>
       </c>
       <c r="C90" s="9">
-        <v>3.7000000000000002E-3</v>
+        <v>0.23325080000000001</v>
       </c>
     </row>
     <row r="91" spans="1:3">
       <c r="A91" s="5" t="s">
-        <v>103</v>
+        <v>110</v>
       </c>
       <c r="B91" s="2">
-        <v>2014</v>
+        <v>2009</v>
       </c>
       <c r="C91" s="9">
-        <v>4.8999999999999998E-3</v>
+        <v>0.24464820000000001</v>
       </c>
     </row>
     <row r="92" spans="1:3">
       <c r="A92" s="5" t="s">
-        <v>183</v>
+        <v>217</v>
       </c>
       <c r="B92" s="2">
-        <v>2014</v>
+        <v>2009</v>
       </c>
       <c r="C92" s="9">
-        <v>9.7000000000000003E-3</v>
+        <v>0.260187</v>
       </c>
     </row>
     <row r="93" spans="1:3">
       <c r="A93" s="5" t="s">
-        <v>108</v>
+        <v>218</v>
       </c>
       <c r="B93" s="2">
-        <v>2014</v>
+        <v>2009</v>
       </c>
       <c r="C93" s="9">
-        <v>1.0699999999999999E-2</v>
+        <v>0.26575209999999999</v>
       </c>
     </row>
     <row r="94" spans="1:3">
       <c r="A94" s="5" t="s">
-        <v>101</v>
+        <v>148</v>
       </c>
       <c r="B94" s="2">
-        <v>2014</v>
+        <v>2009</v>
       </c>
       <c r="C94" s="9">
-        <v>1.1599999999999999E-2</v>
+        <v>0.27524270000000001</v>
       </c>
     </row>
     <row r="95" spans="1:3">
       <c r="A95" s="5" t="s">
-        <v>131</v>
+        <v>174</v>
       </c>
       <c r="B95" s="2">
-        <v>2014</v>
+        <v>2009</v>
       </c>
       <c r="C95" s="9">
-        <v>2.0799999999999999E-2</v>
+        <v>0.28324339999999998</v>
       </c>
     </row>
     <row r="96" spans="1:3">
       <c r="A96" s="5" t="s">
-        <v>196</v>
+        <v>215</v>
       </c>
       <c r="B96" s="2">
-        <v>2014</v>
+        <v>2009</v>
       </c>
       <c r="C96" s="9">
-        <v>2.3599999999999999E-2</v>
+        <v>0.30436079999999999</v>
       </c>
     </row>
     <row r="97" spans="1:3">
       <c r="A97" s="5" t="s">
-        <v>99</v>
+        <v>146</v>
       </c>
       <c r="B97" s="2">
-        <v>2014</v>
+        <v>2009</v>
       </c>
       <c r="C97" s="9">
-        <v>2.8299999999999999E-2</v>
+        <v>0.31811200000000001</v>
       </c>
     </row>
     <row r="98" spans="1:3">
       <c r="A98" s="5" t="s">
-        <v>116</v>
+        <v>123</v>
       </c>
       <c r="B98" s="2">
-        <v>2014</v>
+        <v>2009</v>
       </c>
       <c r="C98" s="9">
-        <v>3.3300000000000003E-2</v>
+        <v>0.32257710000000001</v>
       </c>
     </row>
     <row r="99" spans="1:3">
       <c r="A99" s="5" t="s">
-        <v>112</v>
+        <v>202</v>
       </c>
       <c r="B99" s="2">
-        <v>2014</v>
+        <v>2009</v>
       </c>
       <c r="C99" s="9">
-        <v>3.3599999999999998E-2</v>
+        <v>0.32704949999999999</v>
       </c>
     </row>
     <row r="100" spans="1:3">
       <c r="A100" s="5" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="B100" s="2">
-        <v>2014</v>
+        <v>2009</v>
       </c>
       <c r="C100" s="9">
-        <v>3.4500000000000003E-2</v>
+        <v>0.33949299999999999</v>
       </c>
     </row>
     <row r="101" spans="1:3">
       <c r="A101" s="5" t="s">
-        <v>132</v>
+        <v>183</v>
       </c>
       <c r="B101" s="2">
-        <v>2014</v>
+        <v>2009</v>
       </c>
       <c r="C101" s="9">
-        <v>3.6700000000000003E-2</v>
+        <v>0.3424468</v>
       </c>
     </row>
     <row r="102" spans="1:3">
       <c r="A102" s="5" t="s">
-        <v>176</v>
+        <v>104</v>
       </c>
       <c r="B102" s="2">
-        <v>2014</v>
+        <v>2009</v>
       </c>
       <c r="C102" s="9">
-        <v>3.7499999999999999E-2</v>
+        <v>0.58230440000000006</v>
       </c>
     </row>
     <row r="103" spans="1:3">
       <c r="A103" s="5" t="s">
-        <v>201</v>
+        <v>187</v>
       </c>
       <c r="B103" s="2">
-        <v>2014</v>
+        <v>2009</v>
       </c>
       <c r="C103" s="9">
-        <v>3.8899999999999997E-2</v>
+        <v>0.67780669999999998</v>
       </c>
     </row>
     <row r="104" spans="1:3">
       <c r="A104" s="5" t="s">
-        <v>133</v>
+        <v>13</v>
       </c>
       <c r="B104" s="2">
-        <v>2014</v>
-      </c>
-      <c r="C104" s="9">
-        <v>4.2200000000000001E-2</v>
+        <v>2012</v>
+      </c>
+      <c r="C104" s="8">
+        <v>6.8999999999999999E-3</v>
       </c>
     </row>
     <row r="105" spans="1:3">
       <c r="A105" s="5" t="s">
-        <v>160</v>
+        <v>30</v>
       </c>
       <c r="B105" s="2">
-        <v>2014</v>
-      </c>
-      <c r="C105" s="9">
-        <v>4.24E-2</v>
+        <v>2012</v>
+      </c>
+      <c r="C105" s="8">
+        <v>2.1999999999999999E-2</v>
       </c>
     </row>
     <row r="106" spans="1:3">
       <c r="A106" s="5" t="s">
-        <v>118</v>
+        <v>72</v>
       </c>
       <c r="B106" s="2">
-        <v>2014</v>
-      </c>
-      <c r="C106" s="9">
-        <v>4.4900000000000002E-2</v>
+        <v>2012</v>
+      </c>
+      <c r="C106" s="8">
+        <v>6.4500000000000002E-2</v>
       </c>
     </row>
     <row r="107" spans="1:3">
       <c r="A107" s="5" t="s">
-        <v>117</v>
+        <v>79</v>
       </c>
       <c r="B107" s="2">
-        <v>2014</v>
-      </c>
-      <c r="C107" s="9">
-        <v>4.58E-2</v>
+        <v>2012</v>
+      </c>
+      <c r="C107" s="8">
+        <v>0.10349999999999999</v>
       </c>
     </row>
     <row r="108" spans="1:3">
       <c r="A108" s="5" t="s">
-        <v>121</v>
+        <v>38</v>
       </c>
       <c r="B108" s="2">
-        <v>2014</v>
-      </c>
-      <c r="C108" s="9">
-        <v>4.7699999999999999E-2</v>
+        <v>2012</v>
+      </c>
+      <c r="C108" s="8">
+        <v>0.1047</v>
       </c>
     </row>
     <row r="109" spans="1:3">
       <c r="A109" s="5" t="s">
-        <v>135</v>
+        <v>32</v>
       </c>
       <c r="B109" s="2">
-        <v>2014</v>
-      </c>
-      <c r="C109" s="9">
-        <v>4.9000000000000002E-2</v>
+        <v>2012</v>
+      </c>
+      <c r="C109" s="8">
+        <v>0.1062</v>
       </c>
     </row>
     <row r="110" spans="1:3">
       <c r="A110" s="5" t="s">
-        <v>129</v>
+        <v>88</v>
       </c>
       <c r="B110" s="2">
-        <v>2014</v>
-      </c>
-      <c r="C110" s="9">
-        <v>5.0599999999999999E-2</v>
+        <v>2012</v>
+      </c>
+      <c r="C110" s="8">
+        <v>0.107</v>
       </c>
     </row>
     <row r="111" spans="1:3">
       <c r="A111" s="5" t="s">
-        <v>156</v>
+        <v>21</v>
       </c>
       <c r="B111" s="2">
-        <v>2014</v>
-      </c>
-      <c r="C111" s="9">
-        <v>5.11E-2</v>
+        <v>2012</v>
+      </c>
+      <c r="C111" s="8">
+        <v>0.10920000000000001</v>
       </c>
     </row>
     <row r="112" spans="1:3">
       <c r="A112" s="5" t="s">
-        <v>165</v>
+        <v>33</v>
       </c>
       <c r="B112" s="2">
-        <v>2014</v>
-      </c>
-      <c r="C112" s="9">
-        <v>5.1299999999999998E-2</v>
+        <v>2012</v>
+      </c>
+      <c r="C112" s="8">
+        <v>0.11169999999999999</v>
       </c>
     </row>
     <row r="113" spans="1:3">
       <c r="A113" s="5" t="s">
-        <v>115</v>
+        <v>36</v>
       </c>
       <c r="B113" s="2">
-        <v>2014</v>
-      </c>
-      <c r="C113" s="9">
-        <v>5.79E-2</v>
+        <v>2012</v>
+      </c>
+      <c r="C113" s="8">
+        <v>0.1158</v>
       </c>
     </row>
     <row r="114" spans="1:3">
       <c r="A114" s="5" t="s">
-        <v>177</v>
+        <v>76</v>
       </c>
       <c r="B114" s="2">
-        <v>2014</v>
-      </c>
-      <c r="C114" s="9">
-        <v>5.8000000000000003E-2</v>
+        <v>2012</v>
+      </c>
+      <c r="C114" s="8">
+        <v>0.11799999999999999</v>
       </c>
     </row>
     <row r="115" spans="1:3">
       <c r="A115" s="5" t="s">
-        <v>186</v>
+        <v>73</v>
       </c>
       <c r="B115" s="2">
-        <v>2014</v>
-      </c>
-      <c r="C115" s="9">
-        <v>5.9900000000000002E-2</v>
+        <v>2012</v>
+      </c>
+      <c r="C115" s="8">
+        <v>0.12</v>
       </c>
     </row>
     <row r="116" spans="1:3">
       <c r="A116" s="5" t="s">
-        <v>180</v>
+        <v>24</v>
       </c>
       <c r="B116" s="2">
-        <v>2014</v>
-      </c>
-      <c r="C116" s="9">
-        <v>6.8599999999999994E-2</v>
+        <v>2012</v>
+      </c>
+      <c r="C116" s="8">
+        <v>0.12130000000000001</v>
       </c>
     </row>
     <row r="117" spans="1:3">
       <c r="A117" s="5" t="s">
-        <v>199</v>
+        <v>52</v>
       </c>
       <c r="B117" s="2">
-        <v>2014</v>
-      </c>
-      <c r="C117" s="9">
-        <v>7.4999999999999997E-2</v>
+        <v>2012</v>
+      </c>
+      <c r="C117" s="8">
+        <v>0.122</v>
       </c>
     </row>
     <row r="118" spans="1:3">
       <c r="A118" s="5" t="s">
-        <v>178</v>
+        <v>17</v>
       </c>
       <c r="B118" s="2">
-        <v>2014</v>
-      </c>
-      <c r="C118" s="9">
-        <v>8.2600000000000007E-2</v>
+        <v>2012</v>
+      </c>
+      <c r="C118" s="8">
+        <v>0.12570000000000001</v>
       </c>
     </row>
     <row r="119" spans="1:3">
       <c r="A119" s="5" t="s">
-        <v>126</v>
+        <v>93</v>
       </c>
       <c r="B119" s="2">
-        <v>2014</v>
-      </c>
-      <c r="C119" s="9">
-        <v>8.6199999999999999E-2</v>
+        <v>2012</v>
+      </c>
+      <c r="C119" s="8">
+        <v>0.1258</v>
       </c>
     </row>
     <row r="120" spans="1:3">
       <c r="A120" s="5" t="s">
-        <v>158</v>
+        <v>63</v>
       </c>
       <c r="B120" s="2">
-        <v>2014</v>
-      </c>
-      <c r="C120" s="9">
-        <v>8.7599999999999997E-2</v>
+        <v>2012</v>
+      </c>
+      <c r="C120" s="8">
+        <v>0.12670000000000001</v>
       </c>
     </row>
     <row r="121" spans="1:3">
       <c r="A121" s="5" t="s">
-        <v>161</v>
+        <v>47</v>
       </c>
       <c r="B121" s="2">
-        <v>2014</v>
-      </c>
-      <c r="C121" s="9">
-        <v>0.1002</v>
+        <v>2012</v>
+      </c>
+      <c r="C121" s="8">
+        <v>0.13109999999999999</v>
       </c>
     </row>
     <row r="122" spans="1:3">
       <c r="A122" s="5" t="s">
-        <v>104</v>
+        <v>34</v>
       </c>
       <c r="B122" s="2">
-        <v>2014</v>
-      </c>
-      <c r="C122" s="9">
-        <v>0.1032</v>
+        <v>2012</v>
+      </c>
+      <c r="C122" s="8">
+        <v>0.13139999999999999</v>
       </c>
     </row>
     <row r="123" spans="1:3">
       <c r="A123" s="5" t="s">
-        <v>167</v>
+        <v>19</v>
       </c>
       <c r="B123" s="2">
-        <v>2014</v>
-      </c>
-      <c r="C123" s="9">
-        <v>0.1052</v>
+        <v>2012</v>
+      </c>
+      <c r="C123" s="8">
+        <v>0.1336</v>
       </c>
     </row>
     <row r="124" spans="1:3">
       <c r="A124" s="5" t="s">
-        <v>193</v>
+        <v>66</v>
       </c>
       <c r="B124" s="2">
-        <v>2014</v>
-      </c>
-      <c r="C124" s="9">
-        <v>0.1056</v>
+        <v>2012</v>
+      </c>
+      <c r="C124" s="8">
+        <v>0.1358</v>
       </c>
     </row>
     <row r="125" spans="1:3">
       <c r="A125" s="5" t="s">
-        <v>146</v>
+        <v>89</v>
       </c>
       <c r="B125" s="2">
-        <v>2014</v>
-      </c>
-      <c r="C125" s="9">
-        <v>0.1074</v>
+        <v>2012</v>
+      </c>
+      <c r="C125" s="8">
+        <v>0.13589999999999999</v>
       </c>
     </row>
     <row r="126" spans="1:3">
       <c r="A126" s="5" t="s">
-        <v>114</v>
+        <v>62</v>
       </c>
       <c r="B126" s="2">
-        <v>2014</v>
-      </c>
-      <c r="C126" s="9">
-        <v>0.1142</v>
+        <v>2012</v>
+      </c>
+      <c r="C126" s="8">
+        <v>0.14299999999999999</v>
       </c>
     </row>
     <row r="127" spans="1:3">
       <c r="A127" s="5" t="s">
-        <v>170</v>
+        <v>20</v>
       </c>
       <c r="B127" s="2">
-        <v>2014</v>
-      </c>
-      <c r="C127" s="9">
-        <v>0.1173</v>
+        <v>2012</v>
+      </c>
+      <c r="C127" s="8">
+        <v>0.14330000000000001</v>
       </c>
     </row>
     <row r="128" spans="1:3">
       <c r="A128" s="5" t="s">
-        <v>152</v>
+        <v>86</v>
       </c>
       <c r="B128" s="2">
-        <v>2014</v>
-      </c>
-      <c r="C128" s="9">
-        <v>0.1196</v>
+        <v>2012</v>
+      </c>
+      <c r="C128" s="8">
+        <v>0.14749999999999999</v>
       </c>
     </row>
     <row r="129" spans="1:3">
       <c r="A129" s="5" t="s">
-        <v>125</v>
+        <v>28</v>
       </c>
       <c r="B129" s="2">
-        <v>2014</v>
-      </c>
-      <c r="C129" s="9">
-        <v>0.13100000000000001</v>
+        <v>2012</v>
+      </c>
+      <c r="C129" s="8">
+        <v>0.1477</v>
       </c>
     </row>
     <row r="130" spans="1:3">
       <c r="A130" s="5" t="s">
-        <v>142</v>
+        <v>91</v>
       </c>
       <c r="B130" s="2">
-        <v>2014</v>
-      </c>
-      <c r="C130" s="9">
-        <v>0.1318</v>
+        <v>2012</v>
+      </c>
+      <c r="C130" s="8">
+        <v>0.1522</v>
       </c>
     </row>
     <row r="131" spans="1:3">
       <c r="A131" s="5" t="s">
-        <v>181</v>
+        <v>74</v>
       </c>
       <c r="B131" s="2">
-        <v>2014</v>
-      </c>
-      <c r="C131" s="9">
-        <v>0.13389999999999999</v>
+        <v>2012</v>
+      </c>
+      <c r="C131" s="8">
+        <v>0.15429999999999999</v>
       </c>
     </row>
     <row r="132" spans="1:3">
       <c r="A132" s="5" t="s">
-        <v>137</v>
+        <v>61</v>
       </c>
       <c r="B132" s="2">
-        <v>2014</v>
-      </c>
-      <c r="C132" s="9">
-        <v>0.13450000000000001</v>
+        <v>2012</v>
+      </c>
+      <c r="C132" s="8">
+        <v>0.16020000000000001</v>
       </c>
     </row>
     <row r="133" spans="1:3">
       <c r="A133" s="5" t="s">
-        <v>150</v>
+        <v>57</v>
       </c>
       <c r="B133" s="2">
-        <v>2014</v>
-      </c>
-      <c r="C133" s="9">
-        <v>0.13500000000000001</v>
+        <v>2012</v>
+      </c>
+      <c r="C133" s="8">
+        <v>0.16789999999999999</v>
       </c>
     </row>
     <row r="134" spans="1:3">
       <c r="A134" s="5" t="s">
-        <v>168</v>
+        <v>46</v>
       </c>
       <c r="B134" s="2">
-        <v>2014</v>
-      </c>
-      <c r="C134" s="9">
-        <v>0.13750000000000001</v>
+        <v>2012</v>
+      </c>
+      <c r="C134" s="8">
+        <v>0.16980000000000001</v>
       </c>
     </row>
     <row r="135" spans="1:3">
       <c r="A135" s="5" t="s">
-        <v>205</v>
+        <v>49</v>
       </c>
       <c r="B135" s="2">
-        <v>2014</v>
-      </c>
-      <c r="C135" s="9">
-        <v>0.13919999999999999</v>
+        <v>2012</v>
+      </c>
+      <c r="C135" s="8">
+        <v>0.17430000000000001</v>
       </c>
     </row>
     <row r="136" spans="1:3">
       <c r="A136" s="5" t="s">
-        <v>191</v>
+        <v>54</v>
       </c>
       <c r="B136" s="2">
-        <v>2014</v>
-      </c>
-      <c r="C136" s="9">
-        <v>0.13930000000000001</v>
+        <v>2012</v>
+      </c>
+      <c r="C136" s="8">
+        <v>0.17610000000000001</v>
       </c>
     </row>
     <row r="137" spans="1:3">
       <c r="A137" s="5" t="s">
-        <v>155</v>
+        <v>51</v>
       </c>
       <c r="B137" s="2">
-        <v>2014</v>
-      </c>
-      <c r="C137" s="9">
-        <v>0.14449999999999999</v>
+        <v>2012</v>
+      </c>
+      <c r="C137" s="8">
+        <v>0.2077</v>
       </c>
     </row>
     <row r="138" spans="1:3">
       <c r="A138" s="5" t="s">
-        <v>145</v>
+        <v>43</v>
       </c>
       <c r="B138" s="2">
-        <v>2014</v>
-      </c>
-      <c r="C138" s="9">
-        <v>0.14660000000000001</v>
+        <v>2012</v>
+      </c>
+      <c r="C138" s="8">
+        <v>0.21279999999999999</v>
       </c>
     </row>
     <row r="139" spans="1:3">
       <c r="A139" s="5" t="s">
-        <v>200</v>
+        <v>67</v>
       </c>
       <c r="B139" s="2">
-        <v>2014</v>
-      </c>
-      <c r="C139" s="9">
-        <v>0.14749999999999999</v>
+        <v>2012</v>
+      </c>
+      <c r="C139" s="8">
+        <v>0.21540000000000001</v>
       </c>
     </row>
     <row r="140" spans="1:3">
       <c r="A140" s="5" t="s">
-        <v>148</v>
+        <v>68</v>
       </c>
       <c r="B140" s="2">
-        <v>2014</v>
-      </c>
-      <c r="C140" s="9">
-        <v>0.1532</v>
+        <v>2012</v>
+      </c>
+      <c r="C140" s="8">
+        <v>0.2167</v>
       </c>
     </row>
     <row r="141" spans="1:3">
       <c r="A141" s="5" t="s">
-        <v>172</v>
+        <v>58</v>
       </c>
       <c r="B141" s="2">
-        <v>2014</v>
-      </c>
-      <c r="C141" s="9">
-        <v>0.1595</v>
+        <v>2012</v>
+      </c>
+      <c r="C141" s="8">
+        <v>0.21779999999999999</v>
       </c>
     </row>
     <row r="142" spans="1:3">
       <c r="A142" s="5" t="s">
-        <v>154</v>
+        <v>64</v>
       </c>
       <c r="B142" s="2">
-        <v>2014</v>
-      </c>
-      <c r="C142" s="9">
-        <v>0.1598</v>
+        <v>2012</v>
+      </c>
+      <c r="C142" s="8">
+        <v>0.22</v>
       </c>
     </row>
     <row r="143" spans="1:3">
       <c r="A143" s="5" t="s">
-        <v>120</v>
+        <v>84</v>
       </c>
       <c r="B143" s="2">
-        <v>2014</v>
-      </c>
-      <c r="C143" s="9">
-        <v>0.16619999999999999</v>
+        <v>2012</v>
+      </c>
+      <c r="C143" s="8">
+        <v>0.22459999999999999</v>
       </c>
     </row>
     <row r="144" spans="1:3">
       <c r="A144" s="5" t="s">
-        <v>107</v>
+        <v>75</v>
       </c>
       <c r="B144" s="2">
-        <v>2014</v>
-      </c>
-      <c r="C144" s="9">
-        <v>0.1719</v>
+        <v>2012</v>
+      </c>
+      <c r="C144" s="8">
+        <v>0.23039999999999999</v>
       </c>
     </row>
     <row r="145" spans="1:3">
       <c r="A145" s="5" t="s">
-        <v>179</v>
+        <v>27</v>
       </c>
       <c r="B145" s="2">
-        <v>2014</v>
-      </c>
-      <c r="C145" s="9">
-        <v>0.17649999999999999</v>
+        <v>2012</v>
+      </c>
+      <c r="C145" s="8">
+        <v>0.23880000000000001</v>
       </c>
     </row>
     <row r="146" spans="1:3">
       <c r="A146" s="5" t="s">
-        <v>195</v>
+        <v>94</v>
       </c>
       <c r="B146" s="2">
-        <v>2014</v>
-      </c>
-      <c r="C146" s="9">
-        <v>0.186</v>
+        <v>2012</v>
+      </c>
+      <c r="C146" s="8">
+        <v>0.23930000000000001</v>
       </c>
     </row>
     <row r="147" spans="1:3">
       <c r="A147" s="5" t="s">
-        <v>202</v>
+        <v>65</v>
       </c>
       <c r="B147" s="2">
-        <v>2014</v>
-      </c>
-      <c r="C147" s="9">
-        <v>0.1865</v>
+        <v>2012</v>
+      </c>
+      <c r="C147" s="8">
+        <v>0.24049999999999999</v>
       </c>
     </row>
     <row r="148" spans="1:3">
       <c r="A148" s="5" t="s">
-        <v>187</v>
+        <v>45</v>
       </c>
       <c r="B148" s="2">
-        <v>2014</v>
-      </c>
-      <c r="C148" s="9">
-        <v>0.18940000000000001</v>
+        <v>2012</v>
+      </c>
+      <c r="C148" s="8">
+        <v>0.24429999999999999</v>
       </c>
     </row>
     <row r="149" spans="1:3">
       <c r="A149" s="5" t="s">
-        <v>182</v>
+        <v>53</v>
       </c>
       <c r="B149" s="2">
-        <v>2014</v>
-      </c>
-      <c r="C149" s="9">
-        <v>0.19850000000000001</v>
+        <v>2012</v>
+      </c>
+      <c r="C149" s="8">
+        <v>0.2487</v>
       </c>
     </row>
     <row r="150" spans="1:3">
       <c r="A150" s="5" t="s">
-        <v>197</v>
+        <v>85</v>
       </c>
       <c r="B150" s="2">
-        <v>2014</v>
-      </c>
-      <c r="C150" s="9">
-        <v>0.1986</v>
+        <v>2012</v>
+      </c>
+      <c r="C150" s="8">
+        <v>0.25209999999999999</v>
       </c>
     </row>
     <row r="151" spans="1:3">
       <c r="A151" s="5" t="s">
-        <v>127</v>
+        <v>60</v>
       </c>
       <c r="B151" s="2">
-        <v>2014</v>
-      </c>
-      <c r="C151" s="9">
-        <v>0.20330000000000001</v>
+        <v>2012</v>
+      </c>
+      <c r="C151" s="8">
+        <v>0.2545</v>
       </c>
     </row>
     <row r="152" spans="1:3">
       <c r="A152" s="5" t="s">
-        <v>140</v>
+        <v>55</v>
       </c>
       <c r="B152" s="2">
-        <v>2014</v>
-      </c>
-      <c r="C152" s="9">
-        <v>0.20349999999999999</v>
+        <v>2012</v>
+      </c>
+      <c r="C152" s="8">
+        <v>0.25990000000000002</v>
       </c>
     </row>
     <row r="153" spans="1:3">
       <c r="A153" s="5" t="s">
-        <v>162</v>
+        <v>42</v>
       </c>
       <c r="B153" s="2">
-        <v>2014</v>
-      </c>
-      <c r="C153" s="9">
-        <v>0.20730000000000001</v>
+        <v>2012</v>
+      </c>
+      <c r="C153" s="8">
+        <v>0.26219999999999999</v>
       </c>
     </row>
     <row r="154" spans="1:3">
       <c r="A154" s="5" t="s">
-        <v>144</v>
+        <v>23</v>
       </c>
       <c r="B154" s="2">
-        <v>2014</v>
-      </c>
-      <c r="C154" s="9">
-        <v>0.21099999999999999</v>
+        <v>2012</v>
+      </c>
+      <c r="C154" s="8">
+        <v>0.27550000000000002</v>
       </c>
     </row>
     <row r="155" spans="1:3">
       <c r="A155" s="5" t="s">
-        <v>189</v>
+        <v>12</v>
       </c>
       <c r="B155" s="2">
-        <v>2014</v>
-      </c>
-      <c r="C155" s="9">
-        <v>0.21190000000000001</v>
+        <v>2012</v>
+      </c>
+      <c r="C155" s="8">
+        <v>0.27929999999999999</v>
       </c>
     </row>
     <row r="156" spans="1:3">
       <c r="A156" s="5" t="s">
-        <v>153</v>
+        <v>80</v>
       </c>
       <c r="B156" s="2">
-        <v>2014</v>
-      </c>
-      <c r="C156" s="9">
-        <v>0.2157</v>
+        <v>2012</v>
+      </c>
+      <c r="C156" s="8">
+        <v>0.27979999999999999</v>
       </c>
     </row>
     <row r="157" spans="1:3">
       <c r="A157" s="5" t="s">
-        <v>198</v>
+        <v>14</v>
       </c>
       <c r="B157" s="2">
-        <v>2014</v>
-      </c>
-      <c r="C157" s="9">
-        <v>0.21629999999999999</v>
+        <v>2012</v>
+      </c>
+      <c r="C157" s="8">
+        <v>0.28539999999999999</v>
       </c>
     </row>
     <row r="158" spans="1:3">
       <c r="A158" s="5" t="s">
-        <v>109</v>
+        <v>71</v>
       </c>
       <c r="B158" s="2">
-        <v>2014</v>
-      </c>
-      <c r="C158" s="9">
-        <v>0.23599999999999999</v>
+        <v>2012</v>
+      </c>
+      <c r="C158" s="8">
+        <v>0.29339999999999999</v>
       </c>
     </row>
     <row r="159" spans="1:3">
       <c r="A159" s="5" t="s">
-        <v>110</v>
+        <v>48</v>
       </c>
       <c r="B159" s="2">
-        <v>2014</v>
-      </c>
-      <c r="C159" s="9">
-        <v>0.24030000000000001</v>
+        <v>2012</v>
+      </c>
+      <c r="C159" s="8">
+        <v>0.30470000000000003</v>
       </c>
     </row>
     <row r="160" spans="1:3">
       <c r="A160" s="5" t="s">
-        <v>136</v>
+        <v>92</v>
       </c>
       <c r="B160" s="2">
-        <v>2014</v>
-      </c>
-      <c r="C160" s="9">
-        <v>0.245</v>
+        <v>2012</v>
+      </c>
+      <c r="C160" s="8">
+        <v>0.30470000000000003</v>
       </c>
     </row>
     <row r="161" spans="1:3">
       <c r="A161" s="5" t="s">
-        <v>106</v>
+        <v>96</v>
       </c>
       <c r="B161" s="2">
-        <v>2014</v>
-      </c>
-      <c r="C161" s="9">
-        <v>0.24759999999999999</v>
+        <v>2012</v>
+      </c>
+      <c r="C161" s="8">
+        <v>0.30499999999999999</v>
       </c>
     </row>
     <row r="162" spans="1:3">
       <c r="A162" s="5" t="s">
-        <v>192</v>
+        <v>50</v>
       </c>
       <c r="B162" s="2">
-        <v>2014</v>
-      </c>
-      <c r="C162" s="9">
-        <v>0.25040000000000001</v>
+        <v>2012</v>
+      </c>
+      <c r="C162" s="8">
+        <v>0.3175</v>
       </c>
     </row>
     <row r="163" spans="1:3">
       <c r="A163" s="5" t="s">
-        <v>130</v>
+        <v>41</v>
       </c>
       <c r="B163" s="2">
-        <v>2014</v>
-      </c>
-      <c r="C163" s="9">
-        <v>0.25369999999999998</v>
+        <v>2012</v>
+      </c>
+      <c r="C163" s="8">
+        <v>0.3382</v>
       </c>
     </row>
     <row r="164" spans="1:3">
       <c r="A164" s="5" t="s">
-        <v>194</v>
+        <v>31</v>
       </c>
       <c r="B164" s="2">
-        <v>2014</v>
-      </c>
-      <c r="C164" s="9">
-        <v>0.255</v>
+        <v>2012</v>
+      </c>
+      <c r="C164" s="8">
+        <v>0.3402</v>
       </c>
     </row>
     <row r="165" spans="1:3">
       <c r="A165" s="5" t="s">
-        <v>149</v>
+        <v>56</v>
       </c>
       <c r="B165" s="2">
-        <v>2014</v>
-      </c>
-      <c r="C165" s="9">
-        <v>0.2631</v>
+        <v>2012</v>
+      </c>
+      <c r="C165" s="8">
+        <v>0.34420000000000001</v>
       </c>
     </row>
     <row r="166" spans="1:3">
       <c r="A166" s="5" t="s">
-        <v>147</v>
+        <v>16</v>
       </c>
       <c r="B166" s="2">
-        <v>2014</v>
-      </c>
-      <c r="C166" s="9">
-        <v>0.26500000000000001</v>
+        <v>2012</v>
+      </c>
+      <c r="C166" s="8">
+        <v>0.35239999999999999</v>
       </c>
     </row>
     <row r="167" spans="1:3">
       <c r="A167" s="5" t="s">
-        <v>113</v>
+        <v>37</v>
       </c>
       <c r="B167" s="2">
-        <v>2014</v>
-      </c>
-      <c r="C167" s="9">
-        <v>0.27800000000000002</v>
+        <v>2012</v>
+      </c>
+      <c r="C167" s="8">
+        <v>0.35360000000000003</v>
       </c>
     </row>
     <row r="168" spans="1:3">
       <c r="A168" s="5" t="s">
-        <v>122</v>
+        <v>35</v>
       </c>
       <c r="B168" s="2">
-        <v>2014</v>
-      </c>
-      <c r="C168" s="9">
-        <v>0.28029999999999999</v>
+        <v>2012</v>
+      </c>
+      <c r="C168" s="8">
+        <v>0.35780000000000001</v>
       </c>
     </row>
     <row r="169" spans="1:3">
       <c r="A169" s="5" t="s">
-        <v>119</v>
+        <v>77</v>
       </c>
       <c r="B169" s="2">
-        <v>2014</v>
-      </c>
-      <c r="C169" s="9">
-        <v>0.28189999999999998</v>
+        <v>2012</v>
+      </c>
+      <c r="C169" s="8">
+        <v>0.36099999999999999</v>
       </c>
     </row>
     <row r="170" spans="1:3">
       <c r="A170" s="5" t="s">
-        <v>157</v>
+        <v>87</v>
       </c>
       <c r="B170" s="2">
-        <v>2014</v>
-      </c>
-      <c r="C170" s="9">
-        <v>0.28970000000000001</v>
+        <v>2012</v>
+      </c>
+      <c r="C170" s="8">
+        <v>0.36120000000000002</v>
       </c>
     </row>
     <row r="171" spans="1:3">
       <c r="A171" s="5" t="s">
-        <v>169</v>
+        <v>15</v>
       </c>
       <c r="B171" s="2">
-        <v>2014</v>
-      </c>
-      <c r="C171" s="9">
-        <v>0.29349999999999998</v>
+        <v>2012</v>
+      </c>
+      <c r="C171" s="8">
+        <v>0.36249999999999999</v>
       </c>
     </row>
     <row r="172" spans="1:3">
       <c r="A172" s="5" t="s">
-        <v>141</v>
+        <v>11</v>
       </c>
       <c r="B172" s="2">
-        <v>2014</v>
-      </c>
-      <c r="C172" s="9">
-        <v>0.29880000000000001</v>
+        <v>2012</v>
+      </c>
+      <c r="C172" s="8">
+        <v>0.36309999999999998</v>
       </c>
     </row>
     <row r="173" spans="1:3">
       <c r="A173" s="5" t="s">
-        <v>175</v>
+        <v>22</v>
       </c>
       <c r="B173" s="2">
-        <v>2014</v>
-      </c>
-      <c r="C173" s="9">
-        <v>0.30130000000000001</v>
+        <v>2012</v>
+      </c>
+      <c r="C173" s="8">
+        <v>0.36919999999999997</v>
       </c>
     </row>
     <row r="174" spans="1:3">
       <c r="A174" s="5" t="s">
-        <v>151</v>
+        <v>25</v>
       </c>
       <c r="B174" s="2">
-        <v>2014</v>
-      </c>
-      <c r="C174" s="9">
-        <v>0.31190000000000001</v>
+        <v>2012</v>
+      </c>
+      <c r="C174" s="8">
+        <v>0.37059999999999998</v>
       </c>
     </row>
     <row r="175" spans="1:3">
       <c r="A175" s="5" t="s">
-        <v>143</v>
+        <v>69</v>
       </c>
       <c r="B175" s="2">
-        <v>2014</v>
-      </c>
-      <c r="C175" s="9">
-        <v>0.3206</v>
+        <v>2012</v>
+      </c>
+      <c r="C175" s="8">
+        <v>0.37219999999999998</v>
       </c>
     </row>
     <row r="176" spans="1:3">
       <c r="A176" s="5" t="s">
-        <v>105</v>
+        <v>90</v>
       </c>
       <c r="B176" s="2">
-        <v>2014</v>
-      </c>
-      <c r="C176" s="9">
-        <v>0.32240000000000002</v>
+        <v>2012</v>
+      </c>
+      <c r="C176" s="8">
+        <v>0.3836</v>
       </c>
     </row>
     <row r="177" spans="1:3">
       <c r="A177" s="5" t="s">
-        <v>171</v>
+        <v>82</v>
       </c>
       <c r="B177" s="2">
-        <v>2014</v>
-      </c>
-      <c r="C177" s="9">
-        <v>0.32290000000000002</v>
+        <v>2012</v>
+      </c>
+      <c r="C177" s="8">
+        <v>0.39150000000000001</v>
       </c>
     </row>
     <row r="178" spans="1:3">
       <c r="A178" s="5" t="s">
-        <v>123</v>
+        <v>83</v>
       </c>
       <c r="B178" s="2">
-        <v>2014</v>
-      </c>
-      <c r="C178" s="9">
-        <v>0.32850000000000001</v>
+        <v>2012</v>
+      </c>
+      <c r="C178" s="8">
+        <v>0.39279999999999998</v>
       </c>
     </row>
     <row r="179" spans="1:3">
       <c r="A179" s="5" t="s">
-        <v>184</v>
+        <v>40</v>
       </c>
       <c r="B179" s="2">
-        <v>2014</v>
-      </c>
-      <c r="C179" s="9">
-        <v>0.372</v>
+        <v>2012</v>
+      </c>
+      <c r="C179" s="8">
+        <v>0.3947</v>
       </c>
     </row>
     <row r="180" spans="1:3">
       <c r="A180" s="5" t="s">
-        <v>159</v>
+        <v>39</v>
       </c>
       <c r="B180" s="2">
-        <v>2014</v>
-      </c>
-      <c r="C180" s="9">
-        <v>0.38279999999999997</v>
+        <v>2012</v>
+      </c>
+      <c r="C180" s="8">
+        <v>0.4289</v>
       </c>
     </row>
     <row r="181" spans="1:3">
       <c r="A181" s="5" t="s">
-        <v>111</v>
+        <v>44</v>
       </c>
       <c r="B181" s="2">
-        <v>2014</v>
-      </c>
-      <c r="C181" s="9">
-        <v>0.39</v>
+        <v>2012</v>
+      </c>
+      <c r="C181" s="8">
+        <v>0.44009999999999999</v>
       </c>
     </row>
     <row r="182" spans="1:3">
       <c r="A182" s="5" t="s">
-        <v>174</v>
+        <v>70</v>
       </c>
       <c r="B182" s="2">
-        <v>2014</v>
-      </c>
-      <c r="C182" s="9">
-        <v>0.3911</v>
+        <v>2012</v>
+      </c>
+      <c r="C182" s="8">
+        <v>0.44219999999999998</v>
       </c>
     </row>
     <row r="183" spans="1:3">
       <c r="A183" s="5" t="s">
-        <v>164</v>
+        <v>26</v>
       </c>
       <c r="B183" s="2">
-        <v>2014</v>
-      </c>
-      <c r="C183" s="9">
-        <v>0.39539999999999997</v>
+        <v>2012</v>
+      </c>
+      <c r="C183" s="8">
+        <v>0.45300000000000001</v>
       </c>
     </row>
     <row r="184" spans="1:3">
       <c r="A184" s="5" t="s">
-        <v>138</v>
+        <v>18</v>
       </c>
       <c r="B184" s="2">
-        <v>2014</v>
-      </c>
-      <c r="C184" s="9">
-        <v>0.4022</v>
+        <v>2012</v>
+      </c>
+      <c r="C184" s="8">
+        <v>0.45669999999999999</v>
       </c>
     </row>
     <row r="185" spans="1:3">
       <c r="A185" s="5" t="s">
-        <v>190</v>
+        <v>78</v>
       </c>
       <c r="B185" s="2">
-        <v>2014</v>
-      </c>
-      <c r="C185" s="9">
-        <v>0.41620000000000001</v>
+        <v>2012</v>
+      </c>
+      <c r="C185" s="8">
+        <v>0.49919999999999998</v>
       </c>
     </row>
     <row r="186" spans="1:3">
       <c r="A186" s="5" t="s">
-        <v>128</v>
+        <v>95</v>
       </c>
       <c r="B186" s="2">
-        <v>2014</v>
-      </c>
-      <c r="C186" s="9">
-        <v>0.42759999999999998</v>
+        <v>2012</v>
+      </c>
+      <c r="C186" s="8">
+        <v>0.50619999999999998</v>
       </c>
     </row>
     <row r="187" spans="1:3">
       <c r="A187" s="5" t="s">
-        <v>134</v>
+        <v>29</v>
       </c>
       <c r="B187" s="2">
-        <v>2014</v>
-      </c>
-      <c r="C187" s="9">
-        <v>0.42799999999999999</v>
+        <v>2012</v>
+      </c>
+      <c r="C187" s="8">
+        <v>0.51339999999999997</v>
       </c>
     </row>
     <row r="188" spans="1:3">
       <c r="A188" s="5" t="s">
-        <v>173</v>
+        <v>81</v>
       </c>
       <c r="B188" s="2">
-        <v>2014</v>
-      </c>
-      <c r="C188" s="9">
-        <v>0.4415</v>
+        <v>2012</v>
+      </c>
+      <c r="C188" s="8">
+        <v>0.52459999999999996</v>
       </c>
     </row>
     <row r="189" spans="1:3">
       <c r="A189" s="5" t="s">
-        <v>204</v>
+        <v>59</v>
       </c>
       <c r="B189" s="2">
-        <v>2014</v>
-      </c>
-      <c r="C189" s="9">
-        <v>0.44890000000000002</v>
+        <v>2012</v>
+      </c>
+      <c r="C189" s="8">
+        <v>0.60109999999999997</v>
       </c>
     </row>
     <row r="190" spans="1:3">
       <c r="A190" s="5" t="s">
-        <v>185</v>
+        <v>97</v>
       </c>
       <c r="B190" s="2">
         <v>2014</v>
       </c>
       <c r="C190" s="9">
-        <v>0.45939999999999998</v>
+        <v>1.6000000000000001E-3</v>
       </c>
     </row>
     <row r="191" spans="1:3">
       <c r="A191" s="5" t="s">
-        <v>124</v>
+        <v>99</v>
       </c>
       <c r="B191" s="2">
         <v>2014</v>
       </c>
       <c r="C191" s="9">
-        <v>0.46650000000000003</v>
+        <v>3.3999999999999998E-3</v>
       </c>
     </row>
     <row r="192" spans="1:3">
       <c r="A192" s="5" t="s">
-        <v>163</v>
+        <v>101</v>
       </c>
       <c r="B192" s="2">
         <v>2014</v>
       </c>
       <c r="C192" s="9">
-        <v>0.51639999999999997</v>
+        <v>3.7000000000000002E-3</v>
       </c>
     </row>
     <row r="193" spans="1:3">
       <c r="A193" s="5" t="s">
-        <v>139</v>
+        <v>102</v>
       </c>
       <c r="B193" s="2">
         <v>2014</v>
       </c>
       <c r="C193" s="9">
-        <v>0.52400000000000002</v>
+        <v>4.8999999999999998E-3</v>
       </c>
     </row>
     <row r="194" spans="1:3">
       <c r="A194" s="5" t="s">
-        <v>188</v>
+        <v>182</v>
       </c>
       <c r="B194" s="2">
         <v>2014</v>
       </c>
       <c r="C194" s="9">
-        <v>0.55500000000000005</v>
+        <v>9.7000000000000003E-3</v>
       </c>
     </row>
     <row r="195" spans="1:3">
       <c r="A195" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="B195" s="2">
+        <v>2014</v>
+      </c>
+      <c r="C195" s="9">
+        <v>1.0699999999999999E-2</v>
+      </c>
+    </row>
+    <row r="196" spans="1:3">
+      <c r="A196" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="B196" s="2">
+        <v>2014</v>
+      </c>
+      <c r="C196" s="9">
+        <v>1.1599999999999999E-2</v>
+      </c>
+    </row>
+    <row r="197" spans="1:3">
+      <c r="A197" s="5" t="s">
+        <v>130</v>
+      </c>
+      <c r="B197" s="2">
+        <v>2014</v>
+      </c>
+      <c r="C197" s="9">
+        <v>2.0799999999999999E-2</v>
+      </c>
+    </row>
+    <row r="198" spans="1:3">
+      <c r="A198" s="5" t="s">
+        <v>195</v>
+      </c>
+      <c r="B198" s="2">
+        <v>2014</v>
+      </c>
+      <c r="C198" s="9">
+        <v>2.3599999999999999E-2</v>
+      </c>
+    </row>
+    <row r="199" spans="1:3">
+      <c r="A199" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="B199" s="2">
+        <v>2014</v>
+      </c>
+      <c r="C199" s="9">
+        <v>2.8299999999999999E-2</v>
+      </c>
+    </row>
+    <row r="200" spans="1:3">
+      <c r="A200" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="B200" s="2">
+        <v>2014</v>
+      </c>
+      <c r="C200" s="9">
+        <v>3.3300000000000003E-2</v>
+      </c>
+    </row>
+    <row r="201" spans="1:3">
+      <c r="A201" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="B201" s="2">
+        <v>2014</v>
+      </c>
+      <c r="C201" s="9">
+        <v>3.3599999999999998E-2</v>
+      </c>
+    </row>
+    <row r="202" spans="1:3">
+      <c r="A202" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="B202" s="2">
+        <v>2014</v>
+      </c>
+      <c r="C202" s="9">
+        <v>3.4500000000000003E-2</v>
+      </c>
+    </row>
+    <row r="203" spans="1:3">
+      <c r="A203" s="5" t="s">
+        <v>131</v>
+      </c>
+      <c r="B203" s="2">
+        <v>2014</v>
+      </c>
+      <c r="C203" s="9">
+        <v>3.6700000000000003E-2</v>
+      </c>
+    </row>
+    <row r="204" spans="1:3">
+      <c r="A204" s="5" t="s">
+        <v>175</v>
+      </c>
+      <c r="B204" s="2">
+        <v>2014</v>
+      </c>
+      <c r="C204" s="9">
+        <v>3.7499999999999999E-2</v>
+      </c>
+    </row>
+    <row r="205" spans="1:3">
+      <c r="A205" s="5" t="s">
+        <v>200</v>
+      </c>
+      <c r="B205" s="2">
+        <v>2014</v>
+      </c>
+      <c r="C205" s="9">
+        <v>3.8899999999999997E-2</v>
+      </c>
+    </row>
+    <row r="206" spans="1:3">
+      <c r="A206" s="5" t="s">
+        <v>132</v>
+      </c>
+      <c r="B206" s="2">
+        <v>2014</v>
+      </c>
+      <c r="C206" s="9">
+        <v>4.2200000000000001E-2</v>
+      </c>
+    </row>
+    <row r="207" spans="1:3">
+      <c r="A207" s="5" t="s">
+        <v>159</v>
+      </c>
+      <c r="B207" s="2">
+        <v>2014</v>
+      </c>
+      <c r="C207" s="9">
+        <v>4.24E-2</v>
+      </c>
+    </row>
+    <row r="208" spans="1:3">
+      <c r="A208" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="B208" s="2">
+        <v>2014</v>
+      </c>
+      <c r="C208" s="9">
+        <v>4.4900000000000002E-2</v>
+      </c>
+    </row>
+    <row r="209" spans="1:3">
+      <c r="A209" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="B209" s="2">
+        <v>2014</v>
+      </c>
+      <c r="C209" s="9">
+        <v>4.58E-2</v>
+      </c>
+    </row>
+    <row r="210" spans="1:3">
+      <c r="A210" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="B210" s="2">
+        <v>2014</v>
+      </c>
+      <c r="C210" s="9">
+        <v>4.7699999999999999E-2</v>
+      </c>
+    </row>
+    <row r="211" spans="1:3">
+      <c r="A211" s="5" t="s">
+        <v>134</v>
+      </c>
+      <c r="B211" s="2">
+        <v>2014</v>
+      </c>
+      <c r="C211" s="9">
+        <v>4.9000000000000002E-2</v>
+      </c>
+    </row>
+    <row r="212" spans="1:3">
+      <c r="A212" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="B212" s="2">
+        <v>2014</v>
+      </c>
+      <c r="C212" s="9">
+        <v>5.0599999999999999E-2</v>
+      </c>
+    </row>
+    <row r="213" spans="1:3">
+      <c r="A213" s="5" t="s">
+        <v>155</v>
+      </c>
+      <c r="B213" s="2">
+        <v>2014</v>
+      </c>
+      <c r="C213" s="9">
+        <v>5.11E-2</v>
+      </c>
+    </row>
+    <row r="214" spans="1:3">
+      <c r="A214" s="5" t="s">
+        <v>164</v>
+      </c>
+      <c r="B214" s="2">
+        <v>2014</v>
+      </c>
+      <c r="C214" s="9">
+        <v>5.1299999999999998E-2</v>
+      </c>
+    </row>
+    <row r="215" spans="1:3">
+      <c r="A215" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="B215" s="2">
+        <v>2014</v>
+      </c>
+      <c r="C215" s="9">
+        <v>5.79E-2</v>
+      </c>
+    </row>
+    <row r="216" spans="1:3">
+      <c r="A216" s="5" t="s">
+        <v>176</v>
+      </c>
+      <c r="B216" s="2">
+        <v>2014</v>
+      </c>
+      <c r="C216" s="9">
+        <v>5.8000000000000003E-2</v>
+      </c>
+    </row>
+    <row r="217" spans="1:3">
+      <c r="A217" s="5" t="s">
+        <v>185</v>
+      </c>
+      <c r="B217" s="2">
+        <v>2014</v>
+      </c>
+      <c r="C217" s="9">
+        <v>5.9900000000000002E-2</v>
+      </c>
+    </row>
+    <row r="218" spans="1:3">
+      <c r="A218" s="5" t="s">
+        <v>179</v>
+      </c>
+      <c r="B218" s="2">
+        <v>2014</v>
+      </c>
+      <c r="C218" s="9">
+        <v>6.8599999999999994E-2</v>
+      </c>
+    </row>
+    <row r="219" spans="1:3">
+      <c r="A219" s="5" t="s">
+        <v>198</v>
+      </c>
+      <c r="B219" s="2">
+        <v>2014</v>
+      </c>
+      <c r="C219" s="9">
+        <v>7.4999999999999997E-2</v>
+      </c>
+    </row>
+    <row r="220" spans="1:3">
+      <c r="A220" s="5" t="s">
+        <v>177</v>
+      </c>
+      <c r="B220" s="2">
+        <v>2014</v>
+      </c>
+      <c r="C220" s="9">
+        <v>8.2600000000000007E-2</v>
+      </c>
+    </row>
+    <row r="221" spans="1:3">
+      <c r="A221" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="B221" s="2">
+        <v>2014</v>
+      </c>
+      <c r="C221" s="9">
+        <v>8.6199999999999999E-2</v>
+      </c>
+    </row>
+    <row r="222" spans="1:3">
+      <c r="A222" s="5" t="s">
+        <v>157</v>
+      </c>
+      <c r="B222" s="2">
+        <v>2014</v>
+      </c>
+      <c r="C222" s="9">
+        <v>8.7599999999999997E-2</v>
+      </c>
+    </row>
+    <row r="223" spans="1:3">
+      <c r="A223" s="5" t="s">
+        <v>160</v>
+      </c>
+      <c r="B223" s="2">
+        <v>2014</v>
+      </c>
+      <c r="C223" s="9">
+        <v>0.1002</v>
+      </c>
+    </row>
+    <row r="224" spans="1:3">
+      <c r="A224" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="B224" s="2">
+        <v>2014</v>
+      </c>
+      <c r="C224" s="9">
+        <v>0.1032</v>
+      </c>
+    </row>
+    <row r="225" spans="1:3">
+      <c r="A225" s="5" t="s">
+        <v>166</v>
+      </c>
+      <c r="B225" s="2">
+        <v>2014</v>
+      </c>
+      <c r="C225" s="9">
+        <v>0.1052</v>
+      </c>
+    </row>
+    <row r="226" spans="1:3">
+      <c r="A226" s="5" t="s">
+        <v>192</v>
+      </c>
+      <c r="B226" s="2">
+        <v>2014</v>
+      </c>
+      <c r="C226" s="9">
+        <v>0.1056</v>
+      </c>
+    </row>
+    <row r="227" spans="1:3">
+      <c r="A227" s="5" t="s">
+        <v>145</v>
+      </c>
+      <c r="B227" s="2">
+        <v>2014</v>
+      </c>
+      <c r="C227" s="9">
+        <v>0.1074</v>
+      </c>
+    </row>
+    <row r="228" spans="1:3">
+      <c r="A228" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="B228" s="2">
+        <v>2014</v>
+      </c>
+      <c r="C228" s="9">
+        <v>0.1142</v>
+      </c>
+    </row>
+    <row r="229" spans="1:3">
+      <c r="A229" s="5" t="s">
+        <v>169</v>
+      </c>
+      <c r="B229" s="2">
+        <v>2014</v>
+      </c>
+      <c r="C229" s="9">
+        <v>0.1173</v>
+      </c>
+    </row>
+    <row r="230" spans="1:3">
+      <c r="A230" s="5" t="s">
+        <v>151</v>
+      </c>
+      <c r="B230" s="2">
+        <v>2014</v>
+      </c>
+      <c r="C230" s="9">
+        <v>0.1196</v>
+      </c>
+    </row>
+    <row r="231" spans="1:3">
+      <c r="A231" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="B231" s="2">
+        <v>2014</v>
+      </c>
+      <c r="C231" s="9">
+        <v>0.13100000000000001</v>
+      </c>
+    </row>
+    <row r="232" spans="1:3">
+      <c r="A232" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="B232" s="2">
+        <v>2014</v>
+      </c>
+      <c r="C232" s="9">
+        <v>0.1318</v>
+      </c>
+    </row>
+    <row r="233" spans="1:3">
+      <c r="A233" s="5" t="s">
+        <v>180</v>
+      </c>
+      <c r="B233" s="2">
+        <v>2014</v>
+      </c>
+      <c r="C233" s="9">
+        <v>0.13389999999999999</v>
+      </c>
+    </row>
+    <row r="234" spans="1:3">
+      <c r="A234" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="B234" s="2">
+        <v>2014</v>
+      </c>
+      <c r="C234" s="9">
+        <v>0.13450000000000001</v>
+      </c>
+    </row>
+    <row r="235" spans="1:3">
+      <c r="A235" s="5" t="s">
+        <v>149</v>
+      </c>
+      <c r="B235" s="2">
+        <v>2014</v>
+      </c>
+      <c r="C235" s="9">
+        <v>0.13500000000000001</v>
+      </c>
+    </row>
+    <row r="236" spans="1:3">
+      <c r="A236" s="5" t="s">
+        <v>167</v>
+      </c>
+      <c r="B236" s="2">
+        <v>2014</v>
+      </c>
+      <c r="C236" s="9">
+        <v>0.13750000000000001</v>
+      </c>
+    </row>
+    <row r="237" spans="1:3">
+      <c r="A237" s="5" t="s">
+        <v>204</v>
+      </c>
+      <c r="B237" s="2">
+        <v>2014</v>
+      </c>
+      <c r="C237" s="9">
+        <v>0.13919999999999999</v>
+      </c>
+    </row>
+    <row r="238" spans="1:3">
+      <c r="A238" s="5" t="s">
+        <v>190</v>
+      </c>
+      <c r="B238" s="2">
+        <v>2014</v>
+      </c>
+      <c r="C238" s="9">
+        <v>0.13930000000000001</v>
+      </c>
+    </row>
+    <row r="239" spans="1:3">
+      <c r="A239" s="5" t="s">
+        <v>154</v>
+      </c>
+      <c r="B239" s="2">
+        <v>2014</v>
+      </c>
+      <c r="C239" s="9">
+        <v>0.14449999999999999</v>
+      </c>
+    </row>
+    <row r="240" spans="1:3">
+      <c r="A240" s="5" t="s">
+        <v>144</v>
+      </c>
+      <c r="B240" s="2">
+        <v>2014</v>
+      </c>
+      <c r="C240" s="9">
+        <v>0.14660000000000001</v>
+      </c>
+    </row>
+    <row r="241" spans="1:3">
+      <c r="A241" s="5" t="s">
+        <v>199</v>
+      </c>
+      <c r="B241" s="2">
+        <v>2014</v>
+      </c>
+      <c r="C241" s="9">
+        <v>0.14749999999999999</v>
+      </c>
+    </row>
+    <row r="242" spans="1:3">
+      <c r="A242" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="B242" s="2">
+        <v>2014</v>
+      </c>
+      <c r="C242" s="9">
+        <v>0.1532</v>
+      </c>
+    </row>
+    <row r="243" spans="1:3">
+      <c r="A243" s="5" t="s">
+        <v>171</v>
+      </c>
+      <c r="B243" s="2">
+        <v>2014</v>
+      </c>
+      <c r="C243" s="9">
+        <v>0.1595</v>
+      </c>
+    </row>
+    <row r="244" spans="1:3">
+      <c r="A244" s="5" t="s">
+        <v>153</v>
+      </c>
+      <c r="B244" s="2">
+        <v>2014</v>
+      </c>
+      <c r="C244" s="9">
+        <v>0.1598</v>
+      </c>
+    </row>
+    <row r="245" spans="1:3">
+      <c r="A245" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="B245" s="2">
+        <v>2014</v>
+      </c>
+      <c r="C245" s="9">
+        <v>0.16619999999999999</v>
+      </c>
+    </row>
+    <row r="246" spans="1:3">
+      <c r="A246" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="B246" s="2">
+        <v>2014</v>
+      </c>
+      <c r="C246" s="9">
+        <v>0.1719</v>
+      </c>
+    </row>
+    <row r="247" spans="1:3">
+      <c r="A247" s="5" t="s">
+        <v>178</v>
+      </c>
+      <c r="B247" s="2">
+        <v>2014</v>
+      </c>
+      <c r="C247" s="9">
+        <v>0.17649999999999999</v>
+      </c>
+    </row>
+    <row r="248" spans="1:3">
+      <c r="A248" s="5" t="s">
+        <v>194</v>
+      </c>
+      <c r="B248" s="2">
+        <v>2014</v>
+      </c>
+      <c r="C248" s="9">
+        <v>0.186</v>
+      </c>
+    </row>
+    <row r="249" spans="1:3">
+      <c r="A249" s="5" t="s">
+        <v>201</v>
+      </c>
+      <c r="B249" s="2">
+        <v>2014</v>
+      </c>
+      <c r="C249" s="9">
+        <v>0.1865</v>
+      </c>
+    </row>
+    <row r="250" spans="1:3">
+      <c r="A250" s="5" t="s">
+        <v>186</v>
+      </c>
+      <c r="B250" s="2">
+        <v>2014</v>
+      </c>
+      <c r="C250" s="9">
+        <v>0.18940000000000001</v>
+      </c>
+    </row>
+    <row r="251" spans="1:3">
+      <c r="A251" s="5" t="s">
+        <v>181</v>
+      </c>
+      <c r="B251" s="2">
+        <v>2014</v>
+      </c>
+      <c r="C251" s="9">
+        <v>0.19850000000000001</v>
+      </c>
+    </row>
+    <row r="252" spans="1:3">
+      <c r="A252" s="5" t="s">
+        <v>196</v>
+      </c>
+      <c r="B252" s="2">
+        <v>2014</v>
+      </c>
+      <c r="C252" s="9">
+        <v>0.1986</v>
+      </c>
+    </row>
+    <row r="253" spans="1:3">
+      <c r="A253" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="B253" s="2">
+        <v>2014</v>
+      </c>
+      <c r="C253" s="9">
+        <v>0.20330000000000001</v>
+      </c>
+    </row>
+    <row r="254" spans="1:3">
+      <c r="A254" s="5" t="s">
+        <v>139</v>
+      </c>
+      <c r="B254" s="2">
+        <v>2014</v>
+      </c>
+      <c r="C254" s="9">
+        <v>0.20349999999999999</v>
+      </c>
+    </row>
+    <row r="255" spans="1:3">
+      <c r="A255" s="5" t="s">
+        <v>161</v>
+      </c>
+      <c r="B255" s="2">
+        <v>2014</v>
+      </c>
+      <c r="C255" s="9">
+        <v>0.20730000000000001</v>
+      </c>
+    </row>
+    <row r="256" spans="1:3">
+      <c r="A256" s="5" t="s">
+        <v>143</v>
+      </c>
+      <c r="B256" s="2">
+        <v>2014</v>
+      </c>
+      <c r="C256" s="9">
+        <v>0.21099999999999999</v>
+      </c>
+    </row>
+    <row r="257" spans="1:3">
+      <c r="A257" s="5" t="s">
+        <v>188</v>
+      </c>
+      <c r="B257" s="2">
+        <v>2014</v>
+      </c>
+      <c r="C257" s="9">
+        <v>0.21190000000000001</v>
+      </c>
+    </row>
+    <row r="258" spans="1:3">
+      <c r="A258" s="5" t="s">
+        <v>152</v>
+      </c>
+      <c r="B258" s="2">
+        <v>2014</v>
+      </c>
+      <c r="C258" s="9">
+        <v>0.2157</v>
+      </c>
+    </row>
+    <row r="259" spans="1:3">
+      <c r="A259" s="5" t="s">
+        <v>197</v>
+      </c>
+      <c r="B259" s="2">
+        <v>2014</v>
+      </c>
+      <c r="C259" s="9">
+        <v>0.21629999999999999</v>
+      </c>
+    </row>
+    <row r="260" spans="1:3">
+      <c r="A260" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="B260" s="2">
+        <v>2014</v>
+      </c>
+      <c r="C260" s="9">
+        <v>0.23599999999999999</v>
+      </c>
+    </row>
+    <row r="261" spans="1:3">
+      <c r="A261" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="B261" s="2">
+        <v>2014</v>
+      </c>
+      <c r="C261" s="9">
+        <v>0.24030000000000001</v>
+      </c>
+    </row>
+    <row r="262" spans="1:3">
+      <c r="A262" s="5" t="s">
+        <v>135</v>
+      </c>
+      <c r="B262" s="2">
+        <v>2014</v>
+      </c>
+      <c r="C262" s="9">
+        <v>0.245</v>
+      </c>
+    </row>
+    <row r="263" spans="1:3">
+      <c r="A263" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="B263" s="2">
+        <v>2014</v>
+      </c>
+      <c r="C263" s="9">
+        <v>0.24759999999999999</v>
+      </c>
+    </row>
+    <row r="264" spans="1:3">
+      <c r="A264" s="5" t="s">
+        <v>191</v>
+      </c>
+      <c r="B264" s="2">
+        <v>2014</v>
+      </c>
+      <c r="C264" s="9">
+        <v>0.25040000000000001</v>
+      </c>
+    </row>
+    <row r="265" spans="1:3">
+      <c r="A265" s="5" t="s">
+        <v>129</v>
+      </c>
+      <c r="B265" s="2">
+        <v>2014</v>
+      </c>
+      <c r="C265" s="9">
+        <v>0.25369999999999998</v>
+      </c>
+    </row>
+    <row r="266" spans="1:3">
+      <c r="A266" s="5" t="s">
+        <v>193</v>
+      </c>
+      <c r="B266" s="2">
+        <v>2014</v>
+      </c>
+      <c r="C266" s="9">
+        <v>0.255</v>
+      </c>
+    </row>
+    <row r="267" spans="1:3">
+      <c r="A267" s="5" t="s">
+        <v>148</v>
+      </c>
+      <c r="B267" s="2">
+        <v>2014</v>
+      </c>
+      <c r="C267" s="9">
+        <v>0.2631</v>
+      </c>
+    </row>
+    <row r="268" spans="1:3">
+      <c r="A268" s="5" t="s">
+        <v>146</v>
+      </c>
+      <c r="B268" s="2">
+        <v>2014</v>
+      </c>
+      <c r="C268" s="9">
+        <v>0.26500000000000001</v>
+      </c>
+    </row>
+    <row r="269" spans="1:3">
+      <c r="A269" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="B269" s="2">
+        <v>2014</v>
+      </c>
+      <c r="C269" s="9">
+        <v>0.27800000000000002</v>
+      </c>
+    </row>
+    <row r="270" spans="1:3">
+      <c r="A270" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="B270" s="2">
+        <v>2014</v>
+      </c>
+      <c r="C270" s="9">
+        <v>0.28029999999999999</v>
+      </c>
+    </row>
+    <row r="271" spans="1:3">
+      <c r="A271" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="B271" s="2">
+        <v>2014</v>
+      </c>
+      <c r="C271" s="9">
+        <v>0.28189999999999998</v>
+      </c>
+    </row>
+    <row r="272" spans="1:3">
+      <c r="A272" s="5" t="s">
+        <v>156</v>
+      </c>
+      <c r="B272" s="2">
+        <v>2014</v>
+      </c>
+      <c r="C272" s="9">
+        <v>0.28970000000000001</v>
+      </c>
+    </row>
+    <row r="273" spans="1:3">
+      <c r="A273" s="5" t="s">
+        <v>168</v>
+      </c>
+      <c r="B273" s="2">
+        <v>2014</v>
+      </c>
+      <c r="C273" s="9">
+        <v>0.29349999999999998</v>
+      </c>
+    </row>
+    <row r="274" spans="1:3">
+      <c r="A274" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="B274" s="2">
+        <v>2014</v>
+      </c>
+      <c r="C274" s="9">
+        <v>0.29880000000000001</v>
+      </c>
+    </row>
+    <row r="275" spans="1:3">
+      <c r="A275" s="5" t="s">
+        <v>174</v>
+      </c>
+      <c r="B275" s="2">
+        <v>2014</v>
+      </c>
+      <c r="C275" s="9">
+        <v>0.30130000000000001</v>
+      </c>
+    </row>
+    <row r="276" spans="1:3">
+      <c r="A276" s="5" t="s">
+        <v>150</v>
+      </c>
+      <c r="B276" s="2">
+        <v>2014</v>
+      </c>
+      <c r="C276" s="9">
+        <v>0.31190000000000001</v>
+      </c>
+    </row>
+    <row r="277" spans="1:3">
+      <c r="A277" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="B277" s="2">
+        <v>2014</v>
+      </c>
+      <c r="C277" s="9">
+        <v>0.3206</v>
+      </c>
+    </row>
+    <row r="278" spans="1:3">
+      <c r="A278" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="B278" s="2">
+        <v>2014</v>
+      </c>
+      <c r="C278" s="9">
+        <v>0.32240000000000002</v>
+      </c>
+    </row>
+    <row r="279" spans="1:3">
+      <c r="A279" s="5" t="s">
+        <v>170</v>
+      </c>
+      <c r="B279" s="2">
+        <v>2014</v>
+      </c>
+      <c r="C279" s="9">
+        <v>0.32290000000000002</v>
+      </c>
+    </row>
+    <row r="280" spans="1:3">
+      <c r="A280" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="B280" s="2">
+        <v>2014</v>
+      </c>
+      <c r="C280" s="9">
+        <v>0.32850000000000001</v>
+      </c>
+    </row>
+    <row r="281" spans="1:3">
+      <c r="A281" s="5" t="s">
+        <v>183</v>
+      </c>
+      <c r="B281" s="2">
+        <v>2014</v>
+      </c>
+      <c r="C281" s="9">
+        <v>0.372</v>
+      </c>
+    </row>
+    <row r="282" spans="1:3">
+      <c r="A282" s="5" t="s">
+        <v>158</v>
+      </c>
+      <c r="B282" s="2">
+        <v>2014</v>
+      </c>
+      <c r="C282" s="9">
+        <v>0.38279999999999997</v>
+      </c>
+    </row>
+    <row r="283" spans="1:3">
+      <c r="A283" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="B283" s="2">
+        <v>2014</v>
+      </c>
+      <c r="C283" s="9">
+        <v>0.39</v>
+      </c>
+    </row>
+    <row r="284" spans="1:3">
+      <c r="A284" s="5" t="s">
+        <v>173</v>
+      </c>
+      <c r="B284" s="2">
+        <v>2014</v>
+      </c>
+      <c r="C284" s="9">
+        <v>0.3911</v>
+      </c>
+    </row>
+    <row r="285" spans="1:3">
+      <c r="A285" s="5" t="s">
+        <v>163</v>
+      </c>
+      <c r="B285" s="2">
+        <v>2014</v>
+      </c>
+      <c r="C285" s="9">
+        <v>0.39539999999999997</v>
+      </c>
+    </row>
+    <row r="286" spans="1:3">
+      <c r="A286" s="5" t="s">
+        <v>137</v>
+      </c>
+      <c r="B286" s="2">
+        <v>2014</v>
+      </c>
+      <c r="C286" s="9">
+        <v>0.4022</v>
+      </c>
+    </row>
+    <row r="287" spans="1:3">
+      <c r="A287" s="5" t="s">
+        <v>189</v>
+      </c>
+      <c r="B287" s="2">
+        <v>2014</v>
+      </c>
+      <c r="C287" s="9">
+        <v>0.41620000000000001</v>
+      </c>
+    </row>
+    <row r="288" spans="1:3">
+      <c r="A288" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="B288" s="2">
+        <v>2014</v>
+      </c>
+      <c r="C288" s="9">
+        <v>0.42759999999999998</v>
+      </c>
+    </row>
+    <row r="289" spans="1:3">
+      <c r="A289" s="5" t="s">
+        <v>133</v>
+      </c>
+      <c r="B289" s="2">
+        <v>2014</v>
+      </c>
+      <c r="C289" s="9">
+        <v>0.42799999999999999</v>
+      </c>
+    </row>
+    <row r="290" spans="1:3">
+      <c r="A290" s="5" t="s">
+        <v>172</v>
+      </c>
+      <c r="B290" s="2">
+        <v>2014</v>
+      </c>
+      <c r="C290" s="9">
+        <v>0.4415</v>
+      </c>
+    </row>
+    <row r="291" spans="1:3">
+      <c r="A291" s="5" t="s">
         <v>203</v>
       </c>
-      <c r="B195" s="2">
-        <v>2014</v>
-      </c>
-      <c r="C195" s="9">
+      <c r="B291" s="2">
+        <v>2014</v>
+      </c>
+      <c r="C291" s="9">
+        <v>0.44890000000000002</v>
+      </c>
+    </row>
+    <row r="292" spans="1:3">
+      <c r="A292" s="5" t="s">
+        <v>184</v>
+      </c>
+      <c r="B292" s="2">
+        <v>2014</v>
+      </c>
+      <c r="C292" s="9">
+        <v>0.45939999999999998</v>
+      </c>
+    </row>
+    <row r="293" spans="1:3">
+      <c r="A293" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="B293" s="2">
+        <v>2014</v>
+      </c>
+      <c r="C293" s="9">
+        <v>0.46650000000000003</v>
+      </c>
+    </row>
+    <row r="294" spans="1:3">
+      <c r="A294" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="B294" s="2">
+        <v>2014</v>
+      </c>
+      <c r="C294" s="9">
+        <v>0.51639999999999997</v>
+      </c>
+    </row>
+    <row r="295" spans="1:3">
+      <c r="A295" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="B295" s="2">
+        <v>2014</v>
+      </c>
+      <c r="C295" s="9">
+        <v>0.52400000000000002</v>
+      </c>
+    </row>
+    <row r="296" spans="1:3">
+      <c r="A296" s="5" t="s">
+        <v>187</v>
+      </c>
+      <c r="B296" s="2">
+        <v>2014</v>
+      </c>
+      <c r="C296" s="9">
+        <v>0.55500000000000005</v>
+      </c>
+    </row>
+    <row r="297" spans="1:3">
+      <c r="A297" s="5" t="s">
+        <v>202</v>
+      </c>
+      <c r="B297" s="2">
+        <v>2014</v>
+      </c>
+      <c r="C297" s="9">
         <v>0.56340000000000001</v>
       </c>
     </row>
+    <row r="298" spans="1:3">
+      <c r="C298" s="2"/>
+    </row>
+    <row r="299" spans="1:3">
+      <c r="C299" s="2"/>
+    </row>
+    <row r="301" spans="1:3">
+      <c r="C301" s="2"/>
+    </row>
+    <row r="302" spans="1:3">
+      <c r="C302" s="2"/>
+    </row>
+    <row r="303" spans="1:3">
+      <c r="C303" s="2"/>
+    </row>
+    <row r="304" spans="1:3">
+      <c r="C304" s="2"/>
+    </row>
+    <row r="305" spans="3:3">
+      <c r="C305" s="2"/>
+    </row>
+    <row r="306" spans="3:3">
+      <c r="C306" s="2"/>
+    </row>
+    <row r="307" spans="3:3">
+      <c r="C307" s="2"/>
+    </row>
+    <row r="308" spans="3:3">
+      <c r="C308" s="2"/>
+    </row>
+    <row r="309" spans="3:3">
+      <c r="C309" s="2"/>
+    </row>
+    <row r="310" spans="3:3">
+      <c r="C310" s="2"/>
+    </row>
+    <row r="311" spans="3:3">
+      <c r="C311" s="2"/>
+    </row>
+    <row r="312" spans="3:3">
+      <c r="C312" s="2"/>
+    </row>
+    <row r="313" spans="3:3">
+      <c r="C313" s="2"/>
+    </row>
+    <row r="314" spans="3:3">
+      <c r="C314" s="2"/>
+    </row>
+    <row r="315" spans="3:3">
+      <c r="C315" s="2"/>
+    </row>
+    <row r="316" spans="3:3">
+      <c r="C316" s="2"/>
+    </row>
+    <row r="317" spans="3:3">
+      <c r="C317" s="2"/>
+    </row>
+    <row r="318" spans="3:3">
+      <c r="C318" s="2"/>
+    </row>
+    <row r="319" spans="3:3">
+      <c r="C319" s="2"/>
+    </row>
+    <row r="320" spans="3:3">
+      <c r="C320" s="2"/>
+    </row>
+    <row r="321" spans="3:3">
+      <c r="C321" s="2"/>
+    </row>
+    <row r="322" spans="3:3">
+      <c r="C322" s="2"/>
+    </row>
+    <row r="323" spans="3:3">
+      <c r="C323" s="2"/>
+    </row>
+    <row r="324" spans="3:3">
+      <c r="C324" s="2"/>
+    </row>
+    <row r="325" spans="3:3">
+      <c r="C325" s="2"/>
+    </row>
+    <row r="326" spans="3:3">
+      <c r="C326" s="2"/>
+    </row>
+    <row r="327" spans="3:3">
+      <c r="C327" s="2"/>
+    </row>
+    <row r="328" spans="3:3">
+      <c r="C328" s="2"/>
+    </row>
+    <row r="329" spans="3:3">
+      <c r="C329" s="2"/>
+    </row>
+    <row r="330" spans="3:3">
+      <c r="C330" s="2"/>
+    </row>
+    <row r="331" spans="3:3">
+      <c r="C331" s="2"/>
+    </row>
+    <row r="332" spans="3:3">
+      <c r="C332" s="2"/>
+    </row>
+    <row r="333" spans="3:3">
+      <c r="C333" s="2"/>
+    </row>
+    <row r="334" spans="3:3">
+      <c r="C334" s="2"/>
+    </row>
+    <row r="335" spans="3:3">
+      <c r="C335" s="2"/>
+    </row>
+    <row r="336" spans="3:3">
+      <c r="C336" s="2"/>
+    </row>
+    <row r="337" spans="3:3">
+      <c r="C337" s="2"/>
+    </row>
+    <row r="338" spans="3:3">
+      <c r="C338" s="2"/>
+    </row>
+    <row r="339" spans="3:3">
+      <c r="C339" s="2"/>
+    </row>
+    <row r="340" spans="3:3">
+      <c r="C340" s="2"/>
+    </row>
+    <row r="341" spans="3:3">
+      <c r="C341" s="2"/>
+    </row>
+    <row r="342" spans="3:3">
+      <c r="C342" s="2"/>
+    </row>
+    <row r="343" spans="3:3">
+      <c r="C343" s="2"/>
+    </row>
+    <row r="344" spans="3:3">
+      <c r="C344" s="2"/>
+    </row>
+    <row r="345" spans="3:3">
+      <c r="C345" s="2"/>
+    </row>
+    <row r="346" spans="3:3">
+      <c r="C346" s="2"/>
+    </row>
+    <row r="347" spans="3:3">
+      <c r="C347" s="2"/>
+    </row>
+    <row r="348" spans="3:3">
+      <c r="C348" s="2"/>
+    </row>
+    <row r="349" spans="3:3">
+      <c r="C349" s="2"/>
+    </row>
+    <row r="350" spans="3:3">
+      <c r="C350" s="2"/>
+    </row>
+    <row r="351" spans="3:3">
+      <c r="C351" s="2"/>
+    </row>
+    <row r="352" spans="3:3">
+      <c r="C352" s="2"/>
+    </row>
+    <row r="353" spans="3:3">
+      <c r="C353" s="2"/>
+    </row>
+    <row r="354" spans="3:3">
+      <c r="C354" s="2"/>
+    </row>
+    <row r="355" spans="3:3">
+      <c r="C355" s="2"/>
+    </row>
+    <row r="356" spans="3:3">
+      <c r="C356" s="2"/>
+    </row>
+    <row r="357" spans="3:3">
+      <c r="C357" s="2"/>
+    </row>
+    <row r="358" spans="3:3">
+      <c r="C358" s="2"/>
+    </row>
+    <row r="359" spans="3:3">
+      <c r="C359" s="2"/>
+    </row>
+    <row r="360" spans="3:3">
+      <c r="C360" s="2"/>
+    </row>
+    <row r="361" spans="3:3">
+      <c r="C361" s="2"/>
+    </row>
+    <row r="362" spans="3:3">
+      <c r="C362" s="2"/>
+    </row>
+    <row r="363" spans="3:3">
+      <c r="C363" s="2"/>
+    </row>
+    <row r="364" spans="3:3">
+      <c r="C364" s="2"/>
+    </row>
+    <row r="365" spans="3:3">
+      <c r="C365" s="2"/>
+    </row>
+    <row r="366" spans="3:3">
+      <c r="C366" s="2"/>
+    </row>
+    <row r="367" spans="3:3">
+      <c r="C367" s="2"/>
+    </row>
+    <row r="368" spans="3:3">
+      <c r="C368" s="2"/>
+    </row>
+    <row r="369" spans="3:3">
+      <c r="C369" s="2"/>
+    </row>
+    <row r="370" spans="3:3">
+      <c r="C370" s="2"/>
+    </row>
+    <row r="371" spans="3:3">
+      <c r="C371" s="2"/>
+    </row>
+    <row r="372" spans="3:3">
+      <c r="C372" s="2"/>
+    </row>
+    <row r="373" spans="3:3">
+      <c r="C373" s="2"/>
+    </row>
+    <row r="374" spans="3:3">
+      <c r="C374" s="2"/>
+    </row>
+    <row r="375" spans="3:3">
+      <c r="C375" s="2"/>
+    </row>
+    <row r="376" spans="3:3">
+      <c r="C376" s="2"/>
+    </row>
+    <row r="377" spans="3:3">
+      <c r="C377" s="2"/>
+    </row>
+    <row r="378" spans="3:3">
+      <c r="C378" s="2"/>
+    </row>
+    <row r="379" spans="3:3">
+      <c r="C379" s="2"/>
+    </row>
+    <row r="380" spans="3:3">
+      <c r="C380" s="2"/>
+    </row>
+    <row r="381" spans="3:3">
+      <c r="C381" s="2"/>
+    </row>
+    <row r="382" spans="3:3">
+      <c r="C382" s="2"/>
+    </row>
+    <row r="383" spans="3:3">
+      <c r="C383" s="2"/>
+    </row>
+    <row r="384" spans="3:3">
+      <c r="C384" s="2"/>
+    </row>
+    <row r="385" spans="3:3">
+      <c r="C385" s="2"/>
+    </row>
+    <row r="386" spans="3:3">
+      <c r="C386" s="2"/>
+    </row>
+    <row r="387" spans="3:3">
+      <c r="C387" s="2"/>
+    </row>
+    <row r="388" spans="3:3">
+      <c r="C388" s="2"/>
+    </row>
+    <row r="389" spans="3:3">
+      <c r="C389" s="2"/>
+    </row>
+    <row r="390" spans="3:3">
+      <c r="C390" s="2"/>
+    </row>
+    <row r="391" spans="3:3">
+      <c r="C391" s="2"/>
+    </row>
+    <row r="392" spans="3:3">
+      <c r="C392" s="2"/>
+    </row>
+    <row r="393" spans="3:3">
+      <c r="C393" s="2"/>
+    </row>
+    <row r="394" spans="3:3">
+      <c r="C394" s="2"/>
+    </row>
+    <row r="395" spans="3:3">
+      <c r="C395" s="2"/>
+    </row>
+    <row r="396" spans="3:3">
+      <c r="C396" s="2"/>
+    </row>
+    <row r="397" spans="3:3">
+      <c r="C397" s="2"/>
+    </row>
+    <row r="398" spans="3:3">
+      <c r="C398" s="2"/>
+    </row>
+    <row r="399" spans="3:3">
+      <c r="C399" s="2"/>
+    </row>
+    <row r="400" spans="3:3">
+      <c r="C400" s="2"/>
+    </row>
+    <row r="401" spans="3:3">
+      <c r="C401" s="2"/>
+    </row>
+    <row r="402" spans="3:3">
+      <c r="C402" s="2"/>
+    </row>
+    <row r="403" spans="3:3">
+      <c r="C403" s="2"/>
+    </row>
+    <row r="404" spans="3:3">
+      <c r="C404" s="2"/>
+    </row>
+    <row r="405" spans="3:3">
+      <c r="C405" s="2"/>
+    </row>
+    <row r="406" spans="3:3">
+      <c r="C406" s="2"/>
+    </row>
+    <row r="407" spans="3:3">
+      <c r="C407" s="2"/>
+    </row>
+    <row r="408" spans="3:3">
+      <c r="C408" s="2"/>
+    </row>
+    <row r="409" spans="3:3">
+      <c r="C409" s="2"/>
+    </row>
+    <row r="410" spans="3:3">
+      <c r="C410" s="2"/>
+    </row>
+    <row r="411" spans="3:3">
+      <c r="C411" s="2"/>
+    </row>
+    <row r="412" spans="3:3">
+      <c r="C412" s="2"/>
+    </row>
+    <row r="413" spans="3:3">
+      <c r="C413" s="2"/>
+    </row>
+    <row r="414" spans="3:3">
+      <c r="C414" s="2"/>
+    </row>
+    <row r="415" spans="3:3">
+      <c r="C415" s="2"/>
+    </row>
+    <row r="416" spans="3:3">
+      <c r="C416" s="2"/>
+    </row>
+    <row r="417" spans="3:3">
+      <c r="C417" s="2"/>
+    </row>
+    <row r="418" spans="3:3">
+      <c r="C418" s="2"/>
+    </row>
+    <row r="419" spans="3:3">
+      <c r="C419" s="2"/>
+    </row>
+    <row r="420" spans="3:3">
+      <c r="C420" s="2"/>
+    </row>
+    <row r="421" spans="3:3">
+      <c r="C421" s="2"/>
+    </row>
+    <row r="422" spans="3:3">
+      <c r="C422" s="2"/>
+    </row>
+    <row r="423" spans="3:3">
+      <c r="C423" s="2"/>
+    </row>
+    <row r="424" spans="3:3">
+      <c r="C424" s="2"/>
+    </row>
   </sheetData>
-  <sortState ref="A2:C282">
-    <sortCondition ref="B2:B282"/>
-    <sortCondition ref="C2:C282"/>
+  <sortState ref="A2:C446">
+    <sortCondition ref="B2:B446"/>
+    <sortCondition ref="C2:C446"/>
   </sortState>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -3286,34 +4863,34 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>206</v>
+        <v>225</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" t="s">
         <v>7</v>
-      </c>
-      <c r="B4" t="s">
-        <v>8</v>
       </c>
     </row>
   </sheetData>
@@ -3330,24 +4907,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75"/>
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>2</v>
+        <v>224</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>